<commit_message>
Random fraction of LED value improved
</commit_message>
<xml_diff>
--- a/04_Software/Porting to ESP-IDF.xlsx
+++ b/04_Software/Porting to ESP-IDF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henkj\Documents\GitHub\BedClock\04_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD93F5C-7640-45D0-A5BA-7DE18A174AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA9FDE5-7DB4-46BD-8186-D67238EF32BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{877FF0B8-2AAA-4A03-B534-DDBA6ED9C717}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="194">
   <si>
     <t>Test WS2812 led chain</t>
   </si>
@@ -595,13 +595,64 @@
   <si>
     <t>I (29598) light: I: 42 R: 1 G: 1 B: 0</t>
   </si>
+  <si>
+    <t>58) light: Light manually switched on</t>
+  </si>
+  <si>
+    <t>I (25758) light: R: 1.281 G: 0.990 B: 0.729</t>
+  </si>
+  <si>
+    <t>I (25758) light: R: 2 G: 1 B: 1</t>
+  </si>
+  <si>
+    <t>I (25758) light: R: 1 G: 1 B: 0</t>
+  </si>
+  <si>
+    <t>I (25758) light: R: 1 G: 1 B: 1</t>
+  </si>
+  <si>
+    <t>I (25768) light: R: 2 G: 1 B: 1</t>
+  </si>
+  <si>
+    <t>I (25768) light: R: 1 G: 1 B: 1</t>
+  </si>
+  <si>
+    <t>I (25778) light: R: 1 G: 1 B: 1</t>
+  </si>
+  <si>
+    <t>I (25778) light: R: 2 G: 1 B: 1</t>
+  </si>
+  <si>
+    <t>I (25788) light: R: 2 G: 1 B: 1</t>
+  </si>
+  <si>
+    <t>I (25788) light: R: 1 G: 1 B: 1</t>
+  </si>
+  <si>
+    <t>I (25798) light: R: 1 G: 1 B: 1</t>
+  </si>
+  <si>
+    <t>I (25798) light: R: 1 G: 1 B: 0</t>
+  </si>
+  <si>
+    <t>I (25808) light: R: 1 G: 1 B: 1</t>
+  </si>
+  <si>
+    <t>I (25808) light: R: 1 G: 1 B: 0</t>
+  </si>
+  <si>
+    <t>I (25828) light: R: 1 G: 1 B: 1</t>
+  </si>
+  <si>
+    <t>I (25828) light: R: 2 G: 1 B: 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -692,7 +743,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -2782,7 +2833,7 @@
         <v>110</v>
       </c>
       <c r="D7" t="str">
-        <f t="shared" ref="D2:D11" si="0">A7&amp;"      "&amp;B7</f>
+        <f t="shared" ref="D7:D11" si="0">A7&amp;"      "&amp;B7</f>
         <v>5*60*1000,       // .led_timer = 0</v>
       </c>
       <c r="F7">
@@ -2913,15 +2964,15 @@
         <v>1</v>
       </c>
       <c r="P14">
-        <f>L14/AVERAGE($L14:$N14)</f>
+        <f t="shared" ref="P14:R17" si="2">L14/AVERAGE($L14:$N14)</f>
         <v>1</v>
       </c>
       <c r="Q14">
-        <f>M14/AVERAGE($L14:$N14)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="R14">
-        <f>N14/AVERAGE($L14:$N14)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -2957,15 +3008,15 @@
         <v>0.56862745098039214</v>
       </c>
       <c r="P15">
-        <f>L15/AVERAGE($L15:$N15)</f>
+        <f t="shared" si="2"/>
         <v>1.1787365177195686</v>
       </c>
       <c r="Q15">
-        <f>M15/AVERAGE($L15:$N15)</f>
+        <f t="shared" si="2"/>
         <v>1.1510015408320493</v>
       </c>
       <c r="R15">
-        <f>N15/AVERAGE($L15:$N15)</f>
+        <f t="shared" si="2"/>
         <v>0.67026194144838214</v>
       </c>
     </row>
@@ -2999,15 +3050,15 @@
         <v>145</v>
       </c>
       <c r="P16">
-        <f>L16/AVERAGE($L16:$N16)</f>
+        <f t="shared" si="2"/>
         <v>1.2814070351758795</v>
       </c>
       <c r="Q16">
-        <f>M16/AVERAGE($L16:$N16)</f>
+        <f t="shared" si="2"/>
         <v>0.98994974874371855</v>
       </c>
       <c r="R16">
-        <f>N16/AVERAGE($L16:$N16)</f>
+        <f t="shared" si="2"/>
         <v>0.72864321608040206</v>
       </c>
     </row>
@@ -3041,15 +3092,15 @@
         <v>85</v>
       </c>
       <c r="P17">
-        <f>L17/AVERAGE($L17:$N17)</f>
+        <f t="shared" si="2"/>
         <v>1.8</v>
       </c>
       <c r="Q17">
-        <f>M17/AVERAGE($L17:$N17)</f>
+        <f t="shared" si="2"/>
         <v>0.60000000000000009</v>
       </c>
       <c r="R17">
-        <f>N17/AVERAGE($L17:$N17)</f>
+        <f t="shared" si="2"/>
         <v>0.60000000000000009</v>
       </c>
     </row>
@@ -3087,7 +3138,7 @@
         <v>6.2871668245621765E-2</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" ref="F22:F25" si="2">"    "&amp;TEXT(B22,"0.000")&amp;",  // .led_intensity = "&amp;TEXT(A22,"0")</f>
+        <f t="shared" ref="F22:F25" si="3">"    "&amp;TEXT(B22,"0.000")&amp;",  // .led_intensity = "&amp;TEXT(A22,"0")</f>
         <v xml:space="preserve">    0.063,  // .led_intensity = 1</v>
       </c>
     </row>
@@ -3100,7 +3151,7 @@
         <v>0.15811386671950095</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    0.158,  // .led_intensity = 2</v>
       </c>
     </row>
@@ -3113,7 +3164,7 @@
         <v>0.39763530293683674</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    0.398,  // .led_intensity = 3</v>
       </c>
     </row>
@@ -3126,7 +3177,7 @@
         <v>0.9999997939596843</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v xml:space="preserve">    1.000,  // .led_intensity = 4</v>
       </c>
     </row>
@@ -3277,427 +3328,427 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="str">
-        <f t="shared" ref="A43:A52" si="3">A42&amp;", "&amp;TEXT(B43,"0.00")</f>
+        <f t="shared" ref="A43:A52" si="4">A42&amp;", "&amp;TEXT(B43,"0.00")</f>
         <v>0.00, 0.41, 0.81</v>
       </c>
       <c r="B43" s="12">
-        <f t="shared" ref="B43:B60" si="4">B42+$D$36</f>
+        <f t="shared" ref="B43:B60" si="5">B42+$D$36</f>
         <v>0.81043288469291963</v>
       </c>
       <c r="C43" s="12">
-        <f t="shared" ref="C43:C60" si="5">C42+$D$37</f>
+        <f t="shared" ref="C43:C60" si="6">C42+$D$37</f>
         <v>0.62609913052747113</v>
       </c>
       <c r="D43" s="12">
-        <f t="shared" ref="D43:D60" si="6">D42+$D$38</f>
+        <f t="shared" ref="D43:D60" si="7">D42+$D$38</f>
         <v>0.46083438541362093</v>
       </c>
       <c r="F43" s="13">
-        <f t="shared" ref="F43:F52" si="7">INT(B43)</f>
+        <f t="shared" ref="F43:F52" si="8">INT(B43)</f>
         <v>0</v>
       </c>
       <c r="G43">
-        <f t="shared" ref="G43:G52" si="8">INT(16*MOD(B43,1))</f>
+        <f t="shared" ref="G43:G52" si="9">INT(16*MOD(B43,1))</f>
         <v>12</v>
       </c>
       <c r="I43">
-        <f t="shared" ref="I43:I52" si="9">F43+G43/16</f>
+        <f t="shared" ref="I43:I52" si="10">F43+G43/16</f>
         <v>0.75</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.00, 0.41, 0.81, 1.22</v>
       </c>
       <c r="B44" s="12">
+        <f t="shared" si="5"/>
+        <v>1.2156493270393796</v>
+      </c>
+      <c r="C44" s="12">
+        <f t="shared" si="6"/>
+        <v>0.93914869579120674</v>
+      </c>
+      <c r="D44" s="12">
+        <f t="shared" si="7"/>
+        <v>0.69125157812043136</v>
+      </c>
+      <c r="F44" s="13">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G44">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="10"/>
+        <v>1.1875</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A45" t="str">
         <f t="shared" si="4"/>
-        <v>1.2156493270393796</v>
-      </c>
-      <c r="C44" s="12">
+        <v>0.00, 0.41, 0.81, 1.22, 1.62</v>
+      </c>
+      <c r="B45" s="12">
         <f t="shared" si="5"/>
-        <v>0.93914869579120674</v>
-      </c>
-      <c r="D44" s="12">
+        <v>1.6208657693858393</v>
+      </c>
+      <c r="C45" s="12">
         <f t="shared" si="6"/>
-        <v>0.69125157812043136</v>
-      </c>
-      <c r="F44" s="13">
+        <v>1.2521982610549423</v>
+      </c>
+      <c r="D45" s="12">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="G44">
+        <v>0.92166877082724186</v>
+      </c>
+      <c r="F45" s="13">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="10"/>
+        <v>1.5625</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A46" t="str">
+        <f t="shared" si="4"/>
+        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03</v>
+      </c>
+      <c r="B46" s="12">
+        <f t="shared" si="5"/>
+        <v>2.026082211732299</v>
+      </c>
+      <c r="C46" s="12">
+        <f t="shared" si="6"/>
+        <v>1.5652478263186778</v>
+      </c>
+      <c r="D46" s="12">
+        <f t="shared" si="7"/>
+        <v>1.1520859635340523</v>
+      </c>
+      <c r="F46" s="13">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A47" t="str">
+        <f t="shared" si="4"/>
+        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43</v>
+      </c>
+      <c r="B47" s="12">
+        <f t="shared" si="5"/>
+        <v>2.4312986540787587</v>
+      </c>
+      <c r="C47" s="12">
+        <f t="shared" si="6"/>
+        <v>1.8782973915824133</v>
+      </c>
+      <c r="D47" s="12">
+        <f t="shared" si="7"/>
+        <v>1.3825031562408627</v>
+      </c>
+      <c r="F47" s="13">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <f t="shared" si="9"/>
+        <v>6</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="10"/>
+        <v>2.375</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A48" t="str">
+        <f t="shared" si="4"/>
+        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84</v>
+      </c>
+      <c r="B48" s="12">
+        <f t="shared" si="5"/>
+        <v>2.8365150964252184</v>
+      </c>
+      <c r="C48" s="12">
+        <f t="shared" si="6"/>
+        <v>2.1913469568461488</v>
+      </c>
+      <c r="D48" s="12">
+        <f t="shared" si="7"/>
+        <v>1.6129203489476731</v>
+      </c>
+      <c r="F48" s="13">
+        <f t="shared" si="8"/>
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="10"/>
+        <v>2.8125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A49" t="str">
+        <f t="shared" si="4"/>
+        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24</v>
+      </c>
+      <c r="B49" s="12">
+        <f t="shared" si="5"/>
+        <v>3.2417315387716781</v>
+      </c>
+      <c r="C49" s="12">
+        <f t="shared" si="6"/>
+        <v>2.5043965221098845</v>
+      </c>
+      <c r="D49" s="12">
+        <f t="shared" si="7"/>
+        <v>1.8433375416544835</v>
+      </c>
+      <c r="F49" s="13">
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="I44">
+      <c r="G49">
         <f t="shared" si="9"/>
-        <v>1.1875</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A45" t="str">
-        <f t="shared" si="3"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62</v>
-      </c>
-      <c r="B45" s="12">
+        <v>3</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="10"/>
+        <v>3.1875</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A50" t="str">
         <f t="shared" si="4"/>
-        <v>1.6208657693858393</v>
-      </c>
-      <c r="C45" s="12">
+        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24, 3.65</v>
+      </c>
+      <c r="B50" s="12">
         <f t="shared" si="5"/>
-        <v>1.2521982610549423</v>
-      </c>
-      <c r="D45" s="12">
+        <v>3.6469479811181378</v>
+      </c>
+      <c r="C50" s="12">
         <f t="shared" si="6"/>
-        <v>0.92166877082724186</v>
-      </c>
-      <c r="F45" s="13">
+        <v>2.8174460873736202</v>
+      </c>
+      <c r="D50" s="12">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-      <c r="G45">
-        <f t="shared" si="8"/>
-        <v>9</v>
-      </c>
-      <c r="I45">
-        <f t="shared" si="9"/>
-        <v>1.5625</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A46" t="str">
-        <f t="shared" si="3"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03</v>
-      </c>
-      <c r="B46" s="12">
-        <f t="shared" si="4"/>
-        <v>2.026082211732299</v>
-      </c>
-      <c r="C46" s="12">
-        <f t="shared" si="5"/>
-        <v>1.5652478263186778</v>
-      </c>
-      <c r="D46" s="12">
-        <f t="shared" si="6"/>
-        <v>1.1520859635340523</v>
-      </c>
-      <c r="F46" s="13">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="G46">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <f t="shared" si="9"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A47" t="str">
-        <f t="shared" si="3"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43</v>
-      </c>
-      <c r="B47" s="12">
-        <f t="shared" si="4"/>
-        <v>2.4312986540787587</v>
-      </c>
-      <c r="C47" s="12">
-        <f t="shared" si="5"/>
-        <v>1.8782973915824133</v>
-      </c>
-      <c r="D47" s="12">
-        <f t="shared" si="6"/>
-        <v>1.3825031562408627</v>
-      </c>
-      <c r="F47" s="13">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="G47">
-        <f t="shared" si="8"/>
-        <v>6</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="9"/>
-        <v>2.375</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A48" t="str">
-        <f t="shared" si="3"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84</v>
-      </c>
-      <c r="B48" s="12">
-        <f t="shared" si="4"/>
-        <v>2.8365150964252184</v>
-      </c>
-      <c r="C48" s="12">
-        <f t="shared" si="5"/>
-        <v>2.1913469568461488</v>
-      </c>
-      <c r="D48" s="12">
-        <f t="shared" si="6"/>
-        <v>1.6129203489476731</v>
-      </c>
-      <c r="F48" s="13">
-        <f t="shared" si="7"/>
-        <v>2</v>
-      </c>
-      <c r="G48">
-        <f t="shared" si="8"/>
-        <v>13</v>
-      </c>
-      <c r="I48">
-        <f t="shared" si="9"/>
-        <v>2.8125</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A49" t="str">
-        <f t="shared" si="3"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24</v>
-      </c>
-      <c r="B49" s="12">
-        <f t="shared" si="4"/>
-        <v>3.2417315387716781</v>
-      </c>
-      <c r="C49" s="12">
-        <f t="shared" si="5"/>
-        <v>2.5043965221098845</v>
-      </c>
-      <c r="D49" s="12">
-        <f t="shared" si="6"/>
-        <v>1.8433375416544835</v>
-      </c>
-      <c r="F49" s="13">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="G49">
+        <v>2.0737547343612941</v>
+      </c>
+      <c r="F50" s="13">
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="I49">
+      <c r="G50">
         <f t="shared" si="9"/>
-        <v>3.1875</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A50" t="str">
-        <f t="shared" si="3"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24, 3.65</v>
-      </c>
-      <c r="B50" s="12">
-        <f t="shared" si="4"/>
-        <v>3.6469479811181378</v>
-      </c>
-      <c r="C50" s="12">
-        <f t="shared" si="5"/>
-        <v>2.8174460873736202</v>
-      </c>
-      <c r="D50" s="12">
-        <f t="shared" si="6"/>
-        <v>2.0737547343612941</v>
-      </c>
-      <c r="F50" s="13">
-        <f t="shared" si="7"/>
-        <v>3</v>
-      </c>
-      <c r="G50">
-        <f t="shared" si="8"/>
         <v>10</v>
       </c>
       <c r="I50">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.625</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24, 3.65, 4.05</v>
       </c>
       <c r="B51" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.0521644234645979</v>
       </c>
       <c r="C51" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.130495652637356</v>
       </c>
       <c r="D51" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.3041719270681047</v>
       </c>
       <c r="F51" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="G51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="I51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24, 3.65, 4.05, 4.46</v>
       </c>
       <c r="B52" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.4573808658110581</v>
       </c>
       <c r="C52" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.4435452179010917</v>
       </c>
       <c r="D52" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.5345891197749153</v>
       </c>
       <c r="F52" s="13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="G52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="I52">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.4375</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B53" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.8625973081575182</v>
       </c>
       <c r="C53" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.7565947831648274</v>
       </c>
       <c r="D53" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.7650063124817259</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B54" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.2678137505039784</v>
       </c>
       <c r="C54" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.0696443484285627</v>
       </c>
       <c r="D54" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.9954235051885365</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B55" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.6730301928504385</v>
       </c>
       <c r="C55" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.3826939136922984</v>
       </c>
       <c r="D55" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.2258406978953471</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B56" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.0782466351968987</v>
       </c>
       <c r="C56" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.6957434789560342</v>
       </c>
       <c r="D56" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.4562578906021577</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B57" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.4834630775433588</v>
       </c>
       <c r="C57" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.0087930442197699</v>
       </c>
       <c r="D57" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.6866750833089683</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B58" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.888679519889819</v>
       </c>
       <c r="C58" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.3218426094835056</v>
       </c>
       <c r="D58" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.9170922760157789</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B59" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.2938959622362791</v>
       </c>
       <c r="C59" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.6348921747472414</v>
       </c>
       <c r="D59" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.1475094687225891</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B60" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.6991124045827393</v>
       </c>
       <c r="C60" s="12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.9479417400109771</v>
       </c>
       <c r="D60" s="12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>4.3779266614293997</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="B61" s="12">
-        <f t="shared" ref="B61" si="10">B60+$D$36</f>
+        <f t="shared" ref="B61" si="11">B60+$D$36</f>
         <v>8.1043288469291994</v>
       </c>
       <c r="C61" s="12">
-        <f t="shared" ref="C61" si="11">C60+$D$37</f>
+        <f t="shared" ref="C61" si="12">C60+$D$37</f>
         <v>6.2609913052747128</v>
       </c>
       <c r="D61" s="12">
-        <f t="shared" ref="D61" si="12">D60+$D$38</f>
+        <f t="shared" ref="D61" si="13">D60+$D$38</f>
         <v>4.6083438541362103</v>
       </c>
     </row>
@@ -4064,10 +4115,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD9399F-7175-4AF7-8A2B-38A718F35009}">
-  <dimension ref="A2:F48"/>
+  <dimension ref="A2:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4111,7 +4162,7 @@
       </c>
       <c r="F7">
         <f ca="1">AVERAGE(E8:E23)</f>
-        <v>0.125</v>
+        <v>6.25E-2</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -4120,7 +4171,7 @@
       </c>
       <c r="D8">
         <f ca="1">RAND()</f>
-        <v>0.87052337539550173</v>
+        <v>0.79534334986675947</v>
       </c>
       <c r="E8">
         <f ca="1">IF(D8&gt;=$E$7,0,1)</f>
@@ -4133,7 +4184,7 @@
       </c>
       <c r="D9">
         <f t="shared" ref="D9:D23" ca="1" si="0">RAND()</f>
-        <v>0.99997318160758053</v>
+        <v>0.57180819236266278</v>
       </c>
       <c r="E9">
         <f t="shared" ref="E9:E23" ca="1" si="1">IF(D9&gt;=$E$7,0,1)</f>
@@ -4146,11 +4197,11 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>3.787090656784875E-2</v>
+        <v>0.4956048353672845</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
@@ -4159,7 +4210,7 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53012451916661318</v>
+        <v>0.64444378594425944</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="1"/>
@@ -4172,7 +4223,7 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>0.96452257467143432</v>
+        <v>0.22224331213647319</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="1"/>
@@ -4185,11 +4236,11 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62714519530501434</v>
+        <v>7.9692031806879005E-2</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -4198,17 +4249,17 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>1.077267596677145E-3</v>
+        <v>0.71121411459222172</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>0.25192087955059961</v>
+        <v>0.97604481580659341</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="1"/>
@@ -4218,7 +4269,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91361920716252398</v>
+        <v>0.86293366160840079</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
@@ -4228,7 +4279,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31897995334391649</v>
+        <v>0.42985898335992578</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
@@ -4238,7 +4289,7 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.94987729939125087</v>
+        <v>0.88173439610535809</v>
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
@@ -4248,7 +4299,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73832038508233266</v>
+        <v>0.47308106076830758</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
@@ -4258,7 +4309,7 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.67245587568481346</v>
+        <v>0.80862680393671404</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
@@ -4268,7 +4319,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.71760063066944246</v>
+        <v>0.77949487834763664</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
@@ -4278,7 +4329,7 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.83156450692717088</v>
+        <v>0.59067974748572583</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
@@ -4288,7 +4339,7 @@
     <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="D23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.18247563841590453</v>
+        <v>0.76026987701130966</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="1"/>
@@ -4413,6 +4464,308 @@
     <row r="48" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>176</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>178</v>
+      </c>
+      <c r="B51">
+        <f>AVERAGE(B52:B71)</f>
+        <v>1.25</v>
+      </c>
+      <c r="C51">
+        <f>AVERAGE(C52:C71)</f>
+        <v>1</v>
+      </c>
+      <c r="D51">
+        <f>AVERAGE(D52:D71)</f>
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
+        <v>179</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>180</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
+        <v>181</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>182</v>
+      </c>
+      <c r="B55">
+        <v>2</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>183</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>183</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>184</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
+        <v>185</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>184</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>186</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>187</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>188</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>1</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>188</v>
+      </c>
+      <c r="B64">
+        <v>1</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>189</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>190</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>191</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>190</v>
+      </c>
+      <c r="B68">
+        <v>1</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>192</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>192</v>
+      </c>
+      <c r="B70">
+        <v>1</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>193</v>
+      </c>
+      <c r="B71">
+        <v>2</v>
+      </c>
+      <c r="C71">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved LED control and added display intensity
</commit_message>
<xml_diff>
--- a/04_Software/Porting to ESP-IDF.xlsx
+++ b/04_Software/Porting to ESP-IDF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henkj\Documents\GitHub\BedClock\04_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA9FDE5-7DB4-46BD-8186-D67238EF32BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C95E74-E251-481E-8628-14DA460B3439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{877FF0B8-2AAA-4A03-B534-DDBA6ED9C717}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{877FF0B8-2AAA-4A03-B534-DDBA6ED9C717}"/>
   </bookViews>
   <sheets>
     <sheet name="progress" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="229">
   <si>
     <t>Test WS2812 led chain</t>
   </si>
@@ -503,148 +503,253 @@
     <t>Try using ESP-IDF driver for SSD1306</t>
   </si>
   <si>
-    <t>I (14108) light: Light manually switched on</t>
-  </si>
-  <si>
-    <t>I (14108) light: R: 1.179 G: 1.151 B: 0.670</t>
-  </si>
-  <si>
-    <t>I (14108) light: Red int 1.000 fraction 0.179</t>
-  </si>
-  <si>
-    <t>I (14108) light: Green int 1.000 fraction 0.151</t>
-  </si>
-  <si>
-    <t>I (14118) light: Blue int 0.000 fraction 0.670</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I (14178) display: t1=13457899 t2=13517926 dt=60027. </t>
-  </si>
-  <si>
-    <t>I (14208) main: Main blip</t>
-  </si>
-  <si>
-    <t>I (29058) display: Increase LED color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I (29118) display: t1=28390018 t2=28450283 dt=60265. </t>
-  </si>
-  <si>
-    <t>I (29158) light: R: 1.179 G: 1.151 B: 0.670</t>
-  </si>
-  <si>
-    <t>I (29158) light: Red int 1.000 fraction 0.179</t>
-  </si>
-  <si>
-    <t>I (29158) light: Green int 1.000 fraction 0.151</t>
-  </si>
-  <si>
-    <t>I (29158) light: Blue int 0.000 fraction 0.670</t>
-  </si>
-  <si>
-    <t>I (29238) main: Main blip</t>
-  </si>
-  <si>
-    <t>I (29548) light: Final values for the LEDs:</t>
-  </si>
-  <si>
-    <t>I (29548) light: I: 0 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29548) light: I: 9 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29548) light: I: 18 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29548) light: I: 27 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29568) light: I: 36 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29568) light: I: 45 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29568) light: I: 3 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29568) light: I: 12 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29568) light: I: 21 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29578) light: I: 30 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29578) light: I: 39 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29588) light: I: 6 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29588) light: I: 15 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29598) light: I: 24 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29598) light: I: 33 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (29598) light: I: 42 R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>58) light: Light manually switched on</t>
-  </si>
-  <si>
-    <t>I (25758) light: R: 1.281 G: 0.990 B: 0.729</t>
-  </si>
-  <si>
-    <t>I (25758) light: R: 2 G: 1 B: 1</t>
-  </si>
-  <si>
-    <t>I (25758) light: R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (25758) light: R: 1 G: 1 B: 1</t>
-  </si>
-  <si>
-    <t>I (25768) light: R: 2 G: 1 B: 1</t>
-  </si>
-  <si>
-    <t>I (25768) light: R: 1 G: 1 B: 1</t>
-  </si>
-  <si>
-    <t>I (25778) light: R: 1 G: 1 B: 1</t>
-  </si>
-  <si>
-    <t>I (25778) light: R: 2 G: 1 B: 1</t>
-  </si>
-  <si>
-    <t>I (25788) light: R: 2 G: 1 B: 1</t>
-  </si>
-  <si>
-    <t>I (25788) light: R: 1 G: 1 B: 1</t>
-  </si>
-  <si>
-    <t>I (25798) light: R: 1 G: 1 B: 1</t>
-  </si>
-  <si>
-    <t>I (25798) light: R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (25808) light: R: 1 G: 1 B: 1</t>
-  </si>
-  <si>
-    <t>I (25808) light: R: 1 G: 1 B: 0</t>
-  </si>
-  <si>
-    <t>I (25828) light: R: 1 G: 1 B: 1</t>
-  </si>
-  <si>
-    <t>I (25828) light: R: 2 G: 1 B: 1</t>
+    <t>_x001B_[0;32mI (3228) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (4238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (5238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (5238) main: Auto restart timer 4564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (6238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (7238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (7238) main: Single shot timer_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (8238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (8238) main: Auto restart timer 7564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (9238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (10238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (11238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (11238) main: Auto restart timer 10564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (12238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (13238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (14238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (14238) main: Auto restart timer 13564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (15238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (16238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (17238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (17238) main: Auto restart timer 16564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (18238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (19238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (20238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (20238) main: Auto restart timer 19564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (21238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (22238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (22308) display: Display back to sleep_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (23238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (23238) main: Auto restart timer 22564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (24238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (25238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (26238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (26238) main: Auto restart timer 25564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (27238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (28238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (29238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (29238) main: Auto restart timer 28564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (30238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (31238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (32238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (32238) main: Auto restart timer 31564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (33238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (34238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (35238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (35238) main: Auto restart timer 34564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (36238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (37238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (38238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (38238) main: Auto restart timer 37564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (39238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (40238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (41238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (41238) main: Auto restart timer 40564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (42238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (43238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (44238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (44238) main: Auto restart timer 43564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (45238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (46238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (47238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (47238) main: Auto restart timer 46564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (48238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (49238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (50238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (50238) main: Auto restart timer 49564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (51238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (52238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (53238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (53238) main: Auto restart timer 52564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (54238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (55238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (56238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (56238) main: Auto restart timer 55564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (57238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (58238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (59238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (59238) main: Auto restart timer 58564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (60238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (61238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (62238) main: Main blip_x001B_[0m</t>
+  </si>
+  <si>
+    <t>_x001B_[0;32mI (62238) main: Auto restart timer 61564884_x001B_[0m</t>
+  </si>
+  <si>
+    <t>const uint8_t DISPLAY_INTENSITY[] = {</t>
   </si>
 </sst>
 </file>
@@ -2741,10 +2846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6F3A0C-BCE4-45A2-918D-4AA29D9B0FCD}">
-  <dimension ref="A1:R61"/>
+  <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:F18"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3750,6 +3855,103 @@
       <c r="D61" s="12">
         <f t="shared" ref="D61" si="13">D60+$D$38</f>
         <v>4.6083438541362103</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="B64">
+        <v>2.672340169981581</v>
+      </c>
+      <c r="F64" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A65">
+        <v>0</v>
+      </c>
+      <c r="B65" s="13">
+        <f>B66/$B$64</f>
+        <v>5.0000370298362782</v>
+      </c>
+      <c r="C65" t="str">
+        <f>"0x"&amp;DEC2HEX(B65,2)</f>
+        <v>0x05</v>
+      </c>
+      <c r="F65" s="4" t="str">
+        <f>"    "&amp;C65&amp;" ,    // .display_intensity = "&amp;TEXT(A65,"0")</f>
+        <v xml:space="preserve">    0x05 ,    // .display_intensity = 0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A66">
+        <v>1</v>
+      </c>
+      <c r="B66" s="13">
+        <f>B67/$B$64</f>
+        <v>13.361799806226879</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" ref="C66:C69" si="14">"0x"&amp;DEC2HEX(B66,2)</f>
+        <v>0x0D</v>
+      </c>
+      <c r="F66" s="4" t="str">
+        <f t="shared" ref="F66:F69" si="15">"    "&amp;C66&amp;" ,    // .display_intensity = "&amp;TEXT(A66,"0")</f>
+        <v xml:space="preserve">    0x0D ,    // .display_intensity = 1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>2</v>
+      </c>
+      <c r="B67" s="13">
+        <f>B68/$B$64</f>
+        <v>35.707274365432191</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="14"/>
+        <v>0x23</v>
+      </c>
+      <c r="F67" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">    0x23 ,    // .display_intensity = 2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>3</v>
+      </c>
+      <c r="B68" s="13">
+        <f>B69/$B$64</f>
+        <v>95.421983647298006</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="14"/>
+        <v>0x5F</v>
+      </c>
+      <c r="F68" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">    0x5F ,    // .display_intensity = 3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>4</v>
+      </c>
+      <c r="B69" s="13">
+        <v>255</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="14"/>
+        <v>0xFF</v>
+      </c>
+      <c r="F69" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v xml:space="preserve">    0xFF ,    // .display_intensity = 4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F70" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -4115,284 +4317,116 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD9399F-7175-4AF7-8A2B-38A718F35009}">
-  <dimension ref="A2:F71"/>
+  <dimension ref="A1:H163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="47.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2">
-        <v>255</v>
-      </c>
-      <c r="B2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>149</v>
+      </c>
+      <c r="G7">
+        <v>4564884</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
         <v>150</v>
       </c>
-      <c r="C2">
-        <f>A2*B2/1000</f>
-        <v>38.25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1000</v>
-      </c>
-      <c r="C3">
-        <f>A3*B3/1000</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C4">
-        <f>C2+C3</f>
-        <v>39.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="E7">
-        <v>0.15</v>
-      </c>
-      <c r="F7">
-        <f ca="1">AVERAGE(E8:E23)</f>
-        <v>6.25E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>146</v>
-      </c>
-      <c r="D8">
-        <f ca="1">RAND()</f>
-        <v>0.79534334986675947</v>
-      </c>
-      <c r="E8">
-        <f ca="1">IF(D8&gt;=$E$7,0,1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9">
-        <f t="shared" ref="D9:D23" ca="1" si="0">RAND()</f>
-        <v>0.57180819236266278</v>
-      </c>
-      <c r="E9">
-        <f t="shared" ref="E9:E23" ca="1" si="1">IF(D9&gt;=$E$7,0,1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.4956048353672845</v>
-      </c>
-      <c r="E10">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>149</v>
-      </c>
-      <c r="D11">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.64444378594425944</v>
-      </c>
-      <c r="E11">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.22224331213647319</v>
-      </c>
-      <c r="E12">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>151</v>
-      </c>
-      <c r="D13">
-        <f t="shared" ca="1" si="0"/>
-        <v>7.9692031806879005E-2</v>
-      </c>
-      <c r="E13">
-        <f t="shared" ca="1" si="1"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
         <v>152</v>
       </c>
-      <c r="D14">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.71121411459222172</v>
-      </c>
-      <c r="E14">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="D15">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.97604481580659341</v>
-      </c>
-      <c r="E15">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="D16">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.86293366160840079</v>
-      </c>
-      <c r="E16">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D17">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.42985898335992578</v>
-      </c>
-      <c r="E17">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D18">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.88173439610535809</v>
-      </c>
-      <c r="E18">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D19">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.47308106076830758</v>
-      </c>
-      <c r="E19">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D20">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.80862680393671404</v>
-      </c>
-      <c r="E20">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D21">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.77949487834763664</v>
-      </c>
-      <c r="E21">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D22">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.59067974748572583</v>
-      </c>
-      <c r="E22">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="D23">
-        <f t="shared" ca="1" si="0"/>
-        <v>0.76026987701130966</v>
-      </c>
-      <c r="E23">
-        <f t="shared" ca="1" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>154</v>
+      </c>
+      <c r="G17">
+        <v>7564884</v>
+      </c>
+      <c r="H17">
+        <f>G17-G7</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+        <v>158</v>
+      </c>
+      <c r="G25">
+        <v>10564884</v>
+      </c>
+      <c r="H25">
+        <f>G25-G17</f>
+        <v>3000000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
         <v>162</v>
       </c>
     </row>
@@ -4401,374 +4435,330 @@
         <v>163</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>164</v>
-      </c>
-    </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
         <v>178</v>
       </c>
-      <c r="B51">
-        <f>AVERAGE(B52:B71)</f>
-        <v>1.25</v>
-      </c>
-      <c r="C51">
-        <f>AVERAGE(C52:C71)</f>
-        <v>1</v>
-      </c>
-      <c r="D51">
-        <f>AVERAGE(D52:D71)</f>
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
         <v>179</v>
       </c>
-      <c r="B52">
-        <v>2</v>
-      </c>
-      <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
         <v>180</v>
       </c>
-      <c r="B53">
-        <v>1</v>
-      </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
         <v>181</v>
       </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-      <c r="C54">
-        <v>1</v>
-      </c>
-      <c r="D54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
         <v>182</v>
       </c>
-      <c r="B55">
-        <v>2</v>
-      </c>
-      <c r="C55">
-        <v>1</v>
-      </c>
-      <c r="D55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
         <v>183</v>
       </c>
-      <c r="B56">
-        <v>1</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="D56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>183</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-      <c r="C57">
-        <v>1</v>
-      </c>
-      <c r="D57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
         <v>184</v>
       </c>
-      <c r="B58">
-        <v>1</v>
-      </c>
-      <c r="C58">
-        <v>1</v>
-      </c>
-      <c r="D58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
         <v>185</v>
       </c>
-      <c r="B59">
-        <v>2</v>
-      </c>
-      <c r="C59">
-        <v>1</v>
-      </c>
-      <c r="D59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>184</v>
-      </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A81" t="s">
         <v>186</v>
       </c>
-      <c r="B61">
-        <v>2</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-      <c r="D61">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A83" t="s">
         <v>187</v>
       </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="D62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A85" t="s">
         <v>188</v>
       </c>
-      <c r="B63">
-        <v>1</v>
-      </c>
-      <c r="C63">
-        <v>1</v>
-      </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
-        <v>188</v>
-      </c>
-      <c r="B64">
-        <v>1</v>
-      </c>
-      <c r="C64">
-        <v>1</v>
-      </c>
-      <c r="D64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A87" t="s">
         <v>189</v>
       </c>
-      <c r="B65">
-        <v>1</v>
-      </c>
-      <c r="C65">
-        <v>1</v>
-      </c>
-      <c r="D65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A89" t="s">
         <v>190</v>
       </c>
-      <c r="B66">
-        <v>1</v>
-      </c>
-      <c r="C66">
-        <v>1</v>
-      </c>
-      <c r="D66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A91" t="s">
         <v>191</v>
       </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-      <c r="D67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
-        <v>190</v>
-      </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-      <c r="C68">
-        <v>1</v>
-      </c>
-      <c r="D68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A93" t="s">
         <v>192</v>
       </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-      <c r="C69">
-        <v>1</v>
-      </c>
-      <c r="D69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
-        <v>192</v>
-      </c>
-      <c r="B70">
-        <v>1</v>
-      </c>
-      <c r="C70">
-        <v>1</v>
-      </c>
-      <c r="D70">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A95" t="s">
         <v>193</v>
       </c>
-      <c r="B71">
-        <v>2</v>
-      </c>
-      <c r="C71">
-        <v>1</v>
-      </c>
-      <c r="D71">
-        <v>1</v>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A97" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A99" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A101" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A103" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A105" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A107" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A109" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A111" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A113" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A115" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A117" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A119" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A121" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A123" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A125" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A127" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A129" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A131" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A133" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A135" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A137" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A139" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A141" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A143" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A145" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A147" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A149" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A151" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A153" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A155" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A157" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A159" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A161" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A163" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="I8:J55">
+    <sortCondition ref="I8:I55"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
LVGL working in Bedclock_IDF_V09
</commit_message>
<xml_diff>
--- a/04_Software/Porting to ESP-IDF.xlsx
+++ b/04_Software/Porting to ESP-IDF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henkj\Documents\GitHub\BedClock\04_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C95E74-E251-481E-8628-14DA460B3439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D22015D-E2B1-48C0-8D11-2C3F42EDF290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{877FF0B8-2AAA-4A03-B534-DDBA6ED9C717}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{877FF0B8-2AAA-4A03-B534-DDBA6ED9C717}"/>
   </bookViews>
   <sheets>
     <sheet name="progress" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="231">
   <si>
     <t>Test WS2812 led chain</t>
   </si>
@@ -750,6 +750,12 @@
   </si>
   <si>
     <t>const uint8_t DISPLAY_INTENSITY[] = {</t>
+  </si>
+  <si>
+    <t>Scrolling example LVGL</t>
+  </si>
+  <si>
+    <t>Bedclock_IDF_V12</t>
   </si>
 </sst>
 </file>
@@ -2550,11 +2556,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E3FDF8-1B80-46E7-8A6B-8969C0129D64}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12:G22"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2578,7 +2584,7 @@
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <f>AVERAGE(A4:A1048576)</f>
-        <v>0.55555555555555558</v>
+        <v>0.63157894736842102</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>6</v>
@@ -2713,13 +2719,13 @@
         <v>89</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" ref="G13:G22" si="0">C5&amp;" : "&amp;B5</f>
+        <f t="shared" ref="G13:G24" si="0">C5&amp;" : "&amp;B5</f>
         <v>Bedclock_IDF_V02 : Test SSD1306 OLED screen</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
         <v>145</v>
@@ -2734,7 +2740,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
         <v>4</v>
@@ -2749,93 +2755,92 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>115</v>
+        <v>229</v>
+      </c>
+      <c r="C16" t="s">
+        <v>230</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
         <v>Bedclock_IDF_V05 : Test time sync with timeserver</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="0"/>
         <v>Bedclock_IDF_V06 : Port timer object using esp_timer_get_time() / 1000;</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="0"/>
         <v>Bedclock_IDF_V07 : Test FreeRTOS</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" si="0"/>
         <v>Bedclock_IDF_V08 : Implement multiple parallel processes</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="0"/>
         <v>Bedclock_IDF_V09 : Internal Espressif SSD1306 driver including LVGL</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" si="0"/>
         <v>Bedclock_IDF_V10 : First working version</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
       <c r="G22" t="str">
         <f t="shared" si="0"/>
         <v>Bedclock_IDF_V11 : Try using ESP-IDF driver for SSD1306</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H24">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H25">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="H26">
-        <f>H24/H25</f>
-        <v>3.515625E-2</v>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G23" t="str">
+        <f>C16&amp;" : "&amp;B16</f>
+        <v>Bedclock_IDF_V12 : Scrolling example LVGL</v>
       </c>
     </row>
   </sheetData>
@@ -2846,10 +2851,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6F3A0C-BCE4-45A2-918D-4AA29D9B0FCD}">
-  <dimension ref="A1:R70"/>
+  <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="L62" sqref="L62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3611,7 +3616,7 @@
         <v>2.8125</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" t="str">
         <f t="shared" si="4"/>
         <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24</v>
@@ -3641,7 +3646,7 @@
         <v>3.1875</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" t="str">
         <f t="shared" si="4"/>
         <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24, 3.65</v>
@@ -3671,7 +3676,7 @@
         <v>3.625</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" t="str">
         <f t="shared" si="4"/>
         <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24, 3.65, 4.05</v>
@@ -3701,7 +3706,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" t="str">
         <f t="shared" si="4"/>
         <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24, 3.65, 4.05, 4.46</v>
@@ -3731,7 +3736,7 @@
         <v>4.4375</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B53" s="12">
         <f t="shared" si="5"/>
         <v>4.8625973081575182</v>
@@ -3745,7 +3750,7 @@
         <v>2.7650063124817259</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B54" s="12">
         <f t="shared" si="5"/>
         <v>5.2678137505039784</v>
@@ -3759,7 +3764,7 @@
         <v>2.9954235051885365</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B55" s="12">
         <f t="shared" si="5"/>
         <v>5.6730301928504385</v>
@@ -3773,7 +3778,7 @@
         <v>3.2258406978953471</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B56" s="12">
         <f t="shared" si="5"/>
         <v>6.0782466351968987</v>
@@ -3787,7 +3792,7 @@
         <v>3.4562578906021577</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B57" s="12">
         <f t="shared" si="5"/>
         <v>6.4834630775433588</v>
@@ -3801,7 +3806,7 @@
         <v>3.6866750833089683</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B58" s="12">
         <f t="shared" si="5"/>
         <v>6.888679519889819</v>
@@ -3815,7 +3820,7 @@
         <v>3.9170922760157789</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B59" s="12">
         <f t="shared" si="5"/>
         <v>7.2938959622362791</v>
@@ -3829,7 +3834,7 @@
         <v>4.1475094687225891</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B60" s="12">
         <f t="shared" si="5"/>
         <v>7.6991124045827393</v>
@@ -3843,7 +3848,7 @@
         <v>4.3779266614293997</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B61" s="12">
         <f t="shared" ref="B61" si="11">B60+$D$36</f>
         <v>8.1043288469291994</v>
@@ -3857,9 +3862,15 @@
         <v>4.6083438541362103</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="L62">
+        <f>HEX2DEC("1f")</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B64">
-        <v>2.672340169981581</v>
+        <v>15.967105496833609</v>
       </c>
       <c r="F64" t="s">
         <v>228</v>
@@ -3871,15 +3882,15 @@
       </c>
       <c r="B65" s="13">
         <f>B66/$B$64</f>
-        <v>5.0000370298362782</v>
+        <v>1.0002021665610414</v>
       </c>
       <c r="C65" t="str">
         <f>"0x"&amp;DEC2HEX(B65,2)</f>
-        <v>0x05</v>
+        <v>0x01</v>
       </c>
       <c r="F65" s="4" t="str">
-        <f>"    "&amp;C65&amp;" ,    // .display_intensity = "&amp;TEXT(A65,"0")</f>
-        <v xml:space="preserve">    0x05 ,    // .display_intensity = 0</v>
+        <f>"    "&amp;C65&amp;",    // .display_intensity = "&amp;TEXT(A65,"0")</f>
+        <v xml:space="preserve">    0x01,    // .display_intensity = 0</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
@@ -3888,15 +3899,15 @@
       </c>
       <c r="B66" s="13">
         <f>B67/$B$64</f>
-        <v>13.361799806226879</v>
+        <v>15.970333511641689</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" ref="C66:C69" si="14">"0x"&amp;DEC2HEX(B66,2)</f>
-        <v>0x0D</v>
+        <f t="shared" ref="C66:C67" si="14">"0x"&amp;DEC2HEX(B66,2)</f>
+        <v>0x0F</v>
       </c>
       <c r="F66" s="4" t="str">
-        <f t="shared" ref="F66:F69" si="15">"    "&amp;C66&amp;" ,    // .display_intensity = "&amp;TEXT(A66,"0")</f>
-        <v xml:space="preserve">    0x0D ,    // .display_intensity = 1</v>
+        <f t="shared" ref="F66:F67" si="15">"    "&amp;C66&amp;",    // .display_intensity = "&amp;TEXT(A66,"0")</f>
+        <v xml:space="preserve">    0x0F,    // .display_intensity = 1</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
@@ -3904,53 +3915,19 @@
         <v>2</v>
       </c>
       <c r="B67" s="13">
-        <f>B68/$B$64</f>
-        <v>35.707274365432191</v>
+        <v>255</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="14"/>
-        <v>0x23</v>
+        <v>0xFF</v>
       </c>
       <c r="F67" s="4" t="str">
         <f t="shared" si="15"/>
-        <v xml:space="preserve">    0x23 ,    // .display_intensity = 2</v>
+        <v xml:space="preserve">    0xFF,    // .display_intensity = 2</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A68">
-        <v>3</v>
-      </c>
-      <c r="B68" s="13">
-        <f>B69/$B$64</f>
-        <v>95.421983647298006</v>
-      </c>
-      <c r="C68" t="str">
-        <f t="shared" si="14"/>
-        <v>0x5F</v>
-      </c>
-      <c r="F68" s="4" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    0x5F ,    // .display_intensity = 3</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A69">
-        <v>4</v>
-      </c>
-      <c r="B69" s="13">
-        <v>255</v>
-      </c>
-      <c r="C69" t="str">
-        <f t="shared" si="14"/>
-        <v>0xFF</v>
-      </c>
-      <c r="F69" s="4" t="str">
-        <f t="shared" si="15"/>
-        <v xml:space="preserve">    0xFF ,    // .display_intensity = 4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="F70" s="4" t="s">
+      <c r="F68" s="4" t="s">
         <v>128</v>
       </c>
     </row>

</xml_diff>

<commit_message>
First working version of pixel buffer in Bedclock_IDF_10
</commit_message>
<xml_diff>
--- a/04_Software/Porting to ESP-IDF.xlsx
+++ b/04_Software/Porting to ESP-IDF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henkj\Documents\GitHub\BedClock\04_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D22015D-E2B1-48C0-8D11-2C3F42EDF290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9764F6-79D1-4C47-9AE7-D7A6237C992C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{877FF0B8-2AAA-4A03-B534-DDBA6ED9C717}"/>
+    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{877FF0B8-2AAA-4A03-B534-DDBA6ED9C717}"/>
   </bookViews>
   <sheets>
     <sheet name="progress" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="151">
   <si>
     <t>Test WS2812 led chain</t>
   </si>
@@ -503,252 +503,6 @@
     <t>Try using ESP-IDF driver for SSD1306</t>
   </si>
   <si>
-    <t>_x001B_[0;32mI (3228) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (4238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (5238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (5238) main: Auto restart timer 4564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (6238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (7238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (7238) main: Single shot timer_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (8238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (8238) main: Auto restart timer 7564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (9238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (10238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (11238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (11238) main: Auto restart timer 10564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (12238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (13238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (14238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (14238) main: Auto restart timer 13564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (15238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (16238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (17238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (17238) main: Auto restart timer 16564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (18238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (19238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (20238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (20238) main: Auto restart timer 19564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (21238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (22238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (22308) display: Display back to sleep_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (23238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (23238) main: Auto restart timer 22564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (24238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (25238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (26238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (26238) main: Auto restart timer 25564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (27238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (28238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (29238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (29238) main: Auto restart timer 28564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (30238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (31238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (32238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (32238) main: Auto restart timer 31564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (33238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (34238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (35238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (35238) main: Auto restart timer 34564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (36238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (37238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (38238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (38238) main: Auto restart timer 37564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (39238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (40238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (41238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (41238) main: Auto restart timer 40564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (42238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (43238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (44238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (44238) main: Auto restart timer 43564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (45238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (46238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (47238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (47238) main: Auto restart timer 46564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (48238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (49238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (50238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (50238) main: Auto restart timer 49564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (51238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (52238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (53238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (53238) main: Auto restart timer 52564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (54238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (55238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (56238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (56238) main: Auto restart timer 55564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (57238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (58238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (59238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (59238) main: Auto restart timer 58564884_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (60238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (61238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (62238) main: Main blip_x001B_[0m</t>
-  </si>
-  <si>
-    <t>_x001B_[0;32mI (62238) main: Auto restart timer 61564884_x001B_[0m</t>
-  </si>
-  <si>
     <t>const uint8_t DISPLAY_INTENSITY[] = {</t>
   </si>
   <si>
@@ -756,6 +510,12 @@
   </si>
   <si>
     <t>Bedclock_IDF_V12</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -839,7 +599,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -856,6 +616,9 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2560,7 +2323,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2719,7 +2482,7 @@
         <v>89</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" ref="G13:G24" si="0">C5&amp;" : "&amp;B5</f>
+        <f t="shared" ref="G13:G22" si="0">C5&amp;" : "&amp;B5</f>
         <v>Bedclock_IDF_V02 : Test SSD1306 OLED screen</v>
       </c>
     </row>
@@ -2755,10 +2518,10 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>229</v>
+        <v>147</v>
       </c>
       <c r="C16" t="s">
-        <v>230</v>
+        <v>148</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="0"/>
@@ -2853,8 +2616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6F3A0C-BCE4-45A2-918D-4AA29D9B0FCD}">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="L62" sqref="L62"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3177,20 +2940,20 @@
         <v>3</v>
       </c>
       <c r="B17" s="11">
-        <v>1.8</v>
+        <v>1.5</v>
       </c>
       <c r="C17" s="11">
-        <v>0.60000000000000009</v>
+        <v>0.75</v>
       </c>
       <c r="D17" s="11">
-        <v>0.60000000000000009</v>
+        <v>0.75</v>
       </c>
       <c r="E17" t="s">
         <v>133</v>
       </c>
       <c r="F17" t="str">
         <f>"  { .r = "&amp;TEXT(B17,"0.000")&amp;",  .g = "&amp;TEXT(C17,"0.000")&amp;",  .b = "&amp;TEXT(D17,"0.000")&amp;" },    // "&amp;TEXT(A17,"0")&amp;" = "&amp;E17</f>
-        <v xml:space="preserve">  { .r = 1.800,  .g = 0.600,  .b = 0.600 },    // 3 = Red</v>
+        <v xml:space="preserve">  { .r = 1.500,  .g = 0.750,  .b = 0.750 },    // 3 = Red</v>
       </c>
       <c r="L17">
         <v>255</v>
@@ -3219,12 +2982,40 @@
         <v>128</v>
       </c>
     </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="L19">
+        <v>1.5</v>
+      </c>
+      <c r="M19">
+        <v>0.75</v>
+      </c>
+      <c r="N19">
+        <f>M19</f>
+        <v>0.75</v>
+      </c>
+      <c r="O19">
+        <f>AVERAGE(L19:N19)</f>
+        <v>1</v>
+      </c>
+    </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.45">
       <c r="B20" s="12">
         <v>2.5148667298248704</v>
       </c>
       <c r="F20" t="s">
         <v>135</v>
+      </c>
+      <c r="L20">
+        <f>L19/$O$19</f>
+        <v>1.5</v>
+      </c>
+      <c r="M20">
+        <f>M19/$O$19</f>
+        <v>0.75</v>
+      </c>
+      <c r="N20">
+        <f>N19/$O$19</f>
+        <v>0.75</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.45">
@@ -3873,7 +3664,7 @@
         <v>15.967105496833609</v>
       </c>
       <c r="F64" t="s">
-        <v>228</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
@@ -4294,442 +4085,658 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD9399F-7175-4AF7-8A2B-38A718F35009}">
-  <dimension ref="A1:H163"/>
+  <dimension ref="B2:S17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.46484375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="7" max="7" width="8.73046875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="3.6640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="D2" t="s">
         <v>149</v>
       </c>
-      <c r="G7">
-        <v>4564884</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
+        <f>D3+1</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:X3" si="0">E3+1</f>
+        <v>2</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L3" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M3" s="3">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="N3" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="O3" s="3">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="P3" s="3">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="Q3" s="3">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="R3" s="3">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="S3" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>154</v>
-      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+      <c r="E4" s="14">
+        <f>D4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="14">
+        <f t="shared" ref="F4:S4" si="1">E4</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="14">
+        <v>1</v>
+      </c>
+      <c r="M4" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="N4" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="O4" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="P4" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="R4" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="S4" s="14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="C5" s="3">
+        <f>C4+1</f>
+        <v>1</v>
+      </c>
+      <c r="D5" s="14">
+        <f>D4+2</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="14">
+        <f t="shared" ref="E5:E11" si="2">E4+2</f>
+        <v>2</v>
+      </c>
+      <c r="F5" s="14">
+        <f t="shared" ref="F5:F11" si="3">F4+2</f>
+        <v>2</v>
+      </c>
+      <c r="G5" s="14">
+        <f t="shared" ref="G5:G11" si="4">G4+2</f>
+        <v>2</v>
+      </c>
+      <c r="H5" s="14">
+        <f t="shared" ref="H5:H11" si="5">H4+2</f>
+        <v>2</v>
+      </c>
+      <c r="I5" s="14">
+        <f t="shared" ref="I5:I11" si="6">I4+2</f>
+        <v>2</v>
+      </c>
+      <c r="J5" s="14">
+        <f t="shared" ref="J5:J11" si="7">J4+2</f>
+        <v>2</v>
+      </c>
+      <c r="K5" s="14">
+        <f t="shared" ref="K5:K11" si="8">K4+2</f>
+        <v>2</v>
+      </c>
+      <c r="L5" s="14">
+        <f t="shared" ref="L5:L11" si="9">L4+2</f>
+        <v>3</v>
+      </c>
+      <c r="M5" s="14">
+        <f t="shared" ref="M5:M11" si="10">M4+2</f>
+        <v>3</v>
+      </c>
+      <c r="N5" s="14">
+        <f t="shared" ref="N5:N11" si="11">N4+2</f>
+        <v>3</v>
+      </c>
+      <c r="O5" s="14">
+        <f t="shared" ref="O5:O11" si="12">O4+2</f>
+        <v>3</v>
+      </c>
+      <c r="P5" s="14">
+        <f t="shared" ref="P5:P11" si="13">P4+2</f>
+        <v>3</v>
+      </c>
+      <c r="Q5" s="14">
+        <f t="shared" ref="Q5:Q11" si="14">Q4+2</f>
+        <v>3</v>
+      </c>
+      <c r="R5" s="14">
+        <f t="shared" ref="R5:R11" si="15">R4+2</f>
+        <v>3</v>
+      </c>
+      <c r="S5" s="14">
+        <f t="shared" ref="S5:S11" si="16">S4+2</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="C6" s="3">
+        <f t="shared" ref="C6:C14" si="17">C5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="14">
+        <f t="shared" ref="D6:D11" si="18">D5+2</f>
+        <v>4</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="G6" s="14">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="H6" s="14">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="I6" s="14">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="J6" s="14">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="K6" s="14">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="L6" s="14">
+        <f t="shared" si="9"/>
+        <v>5</v>
+      </c>
+      <c r="M6" s="14">
+        <f t="shared" si="10"/>
+        <v>5</v>
+      </c>
+      <c r="N6" s="14">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="O6" s="14">
+        <f t="shared" si="12"/>
+        <v>5</v>
+      </c>
+      <c r="P6" s="14">
+        <f t="shared" si="13"/>
+        <v>5</v>
+      </c>
+      <c r="Q6" s="14">
+        <f t="shared" si="14"/>
+        <v>5</v>
+      </c>
+      <c r="R6" s="14">
+        <f t="shared" si="15"/>
+        <v>5</v>
+      </c>
+      <c r="S6" s="14">
+        <f t="shared" si="16"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="C7" s="3">
+        <f t="shared" si="17"/>
+        <v>3</v>
+      </c>
+      <c r="D7" s="14">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="E7" s="14">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="F7" s="14">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="G7" s="14">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="H7" s="14">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="I7" s="14">
+        <f t="shared" si="6"/>
+        <v>6</v>
+      </c>
+      <c r="J7" s="14">
+        <f t="shared" si="7"/>
+        <v>6</v>
+      </c>
+      <c r="K7" s="14">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="M7" s="14">
+        <f t="shared" si="10"/>
+        <v>7</v>
+      </c>
+      <c r="N7" s="14">
+        <f t="shared" si="11"/>
+        <v>7</v>
+      </c>
+      <c r="O7" s="14">
+        <f t="shared" si="12"/>
+        <v>7</v>
+      </c>
+      <c r="P7" s="14">
+        <f t="shared" si="13"/>
+        <v>7</v>
+      </c>
+      <c r="Q7" s="14">
+        <f t="shared" si="14"/>
+        <v>7</v>
+      </c>
+      <c r="R7" s="14">
+        <f t="shared" si="15"/>
+        <v>7</v>
+      </c>
+      <c r="S7" s="14">
+        <f t="shared" si="16"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="C8" s="3">
+        <f t="shared" si="17"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="14">
+        <f t="shared" si="18"/>
+        <v>8</v>
+      </c>
+      <c r="E8" s="14">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F8" s="14">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="G8" s="14">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="H8" s="14">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="I8" s="14">
+        <f t="shared" si="6"/>
+        <v>8</v>
+      </c>
+      <c r="J8" s="14">
+        <f t="shared" si="7"/>
+        <v>8</v>
+      </c>
+      <c r="K8" s="14">
+        <f t="shared" si="8"/>
+        <v>8</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" si="9"/>
+        <v>9</v>
+      </c>
+      <c r="M8" s="14">
+        <f t="shared" si="10"/>
+        <v>9</v>
+      </c>
+      <c r="N8" s="14">
+        <f t="shared" si="11"/>
+        <v>9</v>
+      </c>
+      <c r="O8" s="14">
+        <f t="shared" si="12"/>
+        <v>9</v>
+      </c>
+      <c r="P8" s="14">
+        <f t="shared" si="13"/>
+        <v>9</v>
+      </c>
+      <c r="Q8" s="14">
+        <f t="shared" si="14"/>
+        <v>9</v>
+      </c>
+      <c r="R8" s="14">
+        <f t="shared" si="15"/>
+        <v>9</v>
+      </c>
+      <c r="S8" s="14">
+        <f t="shared" si="16"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="C9" s="3">
+        <f t="shared" si="17"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="14">
+        <f t="shared" si="18"/>
+        <v>10</v>
+      </c>
+      <c r="E9" s="14">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="F9" s="14">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G9" s="14">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="H9" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="I9" s="14">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+      <c r="J9" s="14">
+        <f t="shared" si="7"/>
+        <v>10</v>
+      </c>
+      <c r="K9" s="14">
+        <f t="shared" si="8"/>
+        <v>10</v>
+      </c>
+      <c r="L9" s="14">
+        <f t="shared" si="9"/>
+        <v>11</v>
+      </c>
+      <c r="M9" s="14">
+        <f t="shared" si="10"/>
+        <v>11</v>
+      </c>
+      <c r="N9" s="14">
+        <f t="shared" si="11"/>
+        <v>11</v>
+      </c>
+      <c r="O9" s="14">
+        <f t="shared" si="12"/>
+        <v>11</v>
+      </c>
+      <c r="P9" s="14">
+        <f t="shared" si="13"/>
+        <v>11</v>
+      </c>
+      <c r="Q9" s="14">
+        <f t="shared" si="14"/>
+        <v>11</v>
+      </c>
+      <c r="R9" s="14">
+        <f t="shared" si="15"/>
+        <v>11</v>
+      </c>
+      <c r="S9" s="14">
+        <f t="shared" si="16"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="C10" s="3">
+        <f t="shared" si="17"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="14">
+        <f t="shared" si="18"/>
+        <v>12</v>
+      </c>
+      <c r="E10" s="14">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="F10" s="14">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="G10" s="14">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="H10" s="14">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="I10" s="14">
+        <f t="shared" si="6"/>
+        <v>12</v>
+      </c>
+      <c r="J10" s="14">
+        <f t="shared" si="7"/>
+        <v>12</v>
+      </c>
+      <c r="K10" s="14">
+        <f t="shared" si="8"/>
+        <v>12</v>
+      </c>
+      <c r="L10" s="14">
+        <f t="shared" si="9"/>
+        <v>13</v>
+      </c>
+      <c r="M10" s="14">
+        <f t="shared" si="10"/>
+        <v>13</v>
+      </c>
+      <c r="N10" s="14">
+        <f t="shared" si="11"/>
+        <v>13</v>
+      </c>
+      <c r="O10" s="14">
+        <f t="shared" si="12"/>
+        <v>13</v>
+      </c>
+      <c r="P10" s="14">
+        <f t="shared" si="13"/>
+        <v>13</v>
+      </c>
+      <c r="Q10" s="14">
+        <f t="shared" si="14"/>
+        <v>13</v>
+      </c>
+      <c r="R10" s="14">
+        <f t="shared" si="15"/>
+        <v>13</v>
+      </c>
+      <c r="S10" s="14">
+        <f t="shared" si="16"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="C11" s="3">
+        <f t="shared" si="17"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="14">
+        <f t="shared" si="18"/>
+        <v>14</v>
+      </c>
+      <c r="E11" s="14">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="F11" s="14">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="G11" s="14">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="H11" s="14">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="I11" s="14">
+        <f t="shared" si="6"/>
+        <v>14</v>
+      </c>
+      <c r="J11" s="14">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="K11" s="14">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="L11" s="14">
+        <f t="shared" si="9"/>
+        <v>15</v>
+      </c>
+      <c r="M11" s="14">
+        <f t="shared" si="10"/>
+        <v>15</v>
+      </c>
+      <c r="N11" s="14">
+        <f t="shared" si="11"/>
+        <v>15</v>
+      </c>
+      <c r="O11" s="14">
+        <f t="shared" si="12"/>
+        <v>15</v>
+      </c>
+      <c r="P11" s="14">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="Q11" s="14">
+        <f t="shared" si="14"/>
+        <v>15</v>
+      </c>
+      <c r="R11" s="14">
+        <f t="shared" si="15"/>
+        <v>15</v>
+      </c>
+      <c r="S11" s="14">
+        <f t="shared" si="16"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="G15">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.45">
+      <c r="G16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.45">
       <c r="G17">
-        <v>7564884</v>
-      </c>
-      <c r="H17">
-        <f>G17-G7</f>
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>158</v>
-      </c>
-      <c r="G25">
-        <v>10564884</v>
-      </c>
-      <c r="H25">
-        <f>G25-G17</f>
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A71" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A73" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A83" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A85" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A87" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A89" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A91" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A93" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A95" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A97" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A99" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A101" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A103" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A105" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A107" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A109" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A111" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A113" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A115" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A117" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A119" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A121" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A123" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A125" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A127" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A129" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A131" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A133" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A135" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A137" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A139" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A141" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A143" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A145" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A147" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A149" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A151" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A153" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A155" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A157" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A159" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A161" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A163" t="s">
-        <v>227</v>
+        <f>G15*G16</f>
+        <v>512</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Graphical version Bedclock_IDF_V12 working
</commit_message>
<xml_diff>
--- a/04_Software/Porting to ESP-IDF.xlsx
+++ b/04_Software/Porting to ESP-IDF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henkj\Documents\GitHub\BedClock\04_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6738DF-E4B4-4E92-AFBC-282D26754941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3158B7-F326-4442-8AB8-C700573E7B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{877FF0B8-2AAA-4A03-B534-DDBA6ED9C717}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="149">
   <si>
     <t>Test WS2812 led chain</t>
   </si>
@@ -65,18 +65,6 @@
     <t>Implement advanced ssd1306 functions</t>
   </si>
   <si>
-    <t>ssd1306_contrast(&amp;dev, 0xff);</t>
-  </si>
-  <si>
-    <t>ssd1306_software_scroll(&amp;dev, 1, (dev._pages - 1) );</t>
-  </si>
-  <si>
-    <t>Advanced ssd1306 functions:</t>
-  </si>
-  <si>
-    <t>ssd1306_hardware_scroll(&amp;dev, SCROLL_RIGHT);</t>
-  </si>
-  <si>
     <t>T0:</t>
   </si>
   <si>
@@ -270,19 +258,6 @@
   </si>
   <si>
     <t>Bedclock_IDF_V05</t>
-  </si>
-  <si>
-    <r>
-      <t>ssd1306_</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>fadeout(&amp;dev);</t>
-    </r>
   </si>
   <si>
     <t>Document essential settings menu_config</t>
@@ -497,9 +472,6 @@
     <t>const uint8_t DISPLAY_INTENSITY[] = {</t>
   </si>
   <si>
-    <t>Scrolling example LVGL</t>
-  </si>
-  <si>
     <t>Bedclock_IDF_V12</t>
   </si>
   <si>
@@ -522,6 +494,12 @@
   </si>
   <si>
     <t>*/</t>
+  </si>
+  <si>
+    <t>First working version with graphics layout</t>
+  </si>
+  <si>
+    <t>Different projects were created to port the Arduino version to ESP-IDF:</t>
   </si>
 </sst>
 </file>
@@ -531,7 +509,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,11 +541,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Cascadia Mono Light"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Consolas"/>
       <family val="3"/>
     </font>
     <font>
@@ -616,8 +589,8 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2325,11 +2298,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E3FDF8-1B80-46E7-8A6B-8969C0129D64}">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N12" sqref="N12:N23"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2339,330 +2312,324 @@
     <col min="3" max="3" width="15.19921875" customWidth="1"/>
     <col min="4" max="4" width="3.265625" customWidth="1"/>
     <col min="5" max="5" width="2.59765625" customWidth="1"/>
+    <col min="6" max="6" width="58.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="2">
-        <f>AVERAGE(A4:A13)</f>
+        <f>AVERAGE(A5:A14)</f>
         <v>1</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
-        <f>AVERAGE(A4:A1048576)</f>
+        <f>AVERAGE(A5:A1048576)</f>
         <v>0.61111111111111116</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>72</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="2"/>
+      <c r="F3" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" t="str">
+        <f t="shared" ref="F5:F16" si="0">"    "&amp;C5&amp;" : "&amp;B5</f>
+        <v xml:space="preserve">    Bedclock_IDF_V01 : Test WS2812 led chain</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" ref="G5:G16" si="1">"  * `"&amp;C5&amp;"` : "&amp;B5</f>
+        <v xml:space="preserve">  * `Bedclock_IDF_V01` : Test WS2812 led chain</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    Bedclock_IDF_V02 : Test SSD1306 OLED screen</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  * `Bedclock_IDF_V02` : Test SSD1306 OLED screen</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+        <v>70</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    Bedclock_IDF_V03 : Test capacitive touch sensors</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  * `Bedclock_IDF_V03` : Test capacitive touch sensors</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+        <v>67</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    Bedclock_IDF_V04 : Test WiFi</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  * `Bedclock_IDF_V04` : Test WiFi</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+        <v>71</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    Bedclock_IDF_V05 : Test time sync with timeserver</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  * `Bedclock_IDF_V05` : Test time sync with timeserver</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="C10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
+        <v>75</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    Bedclock_IDF_V06 : Port timer object using esp_timer_get_time() / 1000;</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  * `Bedclock_IDF_V06` : Port timer object using esp_timer_get_time() / 1000;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>115</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>82</v>
-      </c>
-      <c r="G11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    Bedclock_IDF_V07 : Test FreeRTOS</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  * `Bedclock_IDF_V07` : Test FreeRTOS</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1">
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>77</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    Bedclock_IDF_V08 : Implement multiple parallel processes</v>
       </c>
       <c r="G12" t="str">
-        <f>"    "&amp;C4&amp;" : "&amp;B4</f>
-        <v xml:space="preserve">    Bedclock_IDF_V01 : Test WS2812 led chain</v>
-      </c>
-      <c r="N12" t="str">
-        <f>"  * `"&amp;C4&amp;"` : "&amp;B4</f>
-        <v xml:space="preserve">  * `Bedclock_IDF_V01` : Test WS2812 led chain</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  * `Bedclock_IDF_V08` : Implement multiple parallel processes</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>149</v>
+        <v>79</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>78</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    Bedclock_IDF_V09 : Internal Espressif SSD1306 driver including LVGL</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" ref="G13:G24" si="0">"    "&amp;C5&amp;" : "&amp;B5</f>
-        <v xml:space="preserve">    Bedclock_IDF_V02 : Test SSD1306 OLED screen</v>
-      </c>
-      <c r="N13" t="str">
-        <f t="shared" ref="N13:N23" si="1">"  * `"&amp;C5&amp;"` : "&amp;B5</f>
-        <v xml:space="preserve">  * `Bedclock_IDF_V02` : Test SSD1306 OLED screen</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  * `Bedclock_IDF_V09` : Internal Espressif SSD1306 driver including LVGL</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>99</v>
+        <v>82</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    Bedclock_IDF_V10 : First working version of application</v>
       </c>
       <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve">  * `Bedclock_IDF_V10` : First working version of application</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>142</v>
+      </c>
+      <c r="C15" t="s">
+        <v>94</v>
+      </c>
+      <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">    Bedclock_IDF_V03 : Test capacitive touch sensors</v>
-      </c>
-      <c r="N14" t="str">
+        <v xml:space="preserve">    Bedclock_IDF_V11 : First working version of pixel buffer</v>
+      </c>
+      <c r="G15" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  * `Bedclock_IDF_V03` : Test capacitive touch sensors</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A15" s="1">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>144</v>
-      </c>
-      <c r="C15" t="s">
-        <v>145</v>
-      </c>
-      <c r="G15" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    Bedclock_IDF_V04 : Test WiFi</v>
-      </c>
-      <c r="N15" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  * `Bedclock_IDF_V04` : Test WiFi</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">  * `Bedclock_IDF_V11` : First working version of pixel buffer</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1">
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>113</v>
+        <v>147</v>
+      </c>
+      <c r="C16" t="s">
+        <v>139</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">    Bedclock_IDF_V12 : First working version with graphics layout</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    Bedclock_IDF_V05 : Test time sync with timeserver</v>
-      </c>
-      <c r="N16" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">  * `Bedclock_IDF_V05` : Test time sync with timeserver</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+        <v xml:space="preserve">  * `Bedclock_IDF_V12` : First working version with graphics layout</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1">
         <v>0</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
-      </c>
-      <c r="G17" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    Bedclock_IDF_V06 : Port timer object using esp_timer_get_time() / 1000;</v>
-      </c>
-      <c r="N17" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  * `Bedclock_IDF_V06` : Port timer object using esp_timer_get_time() / 1000;</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+        <v>108</v>
+      </c>
+      <c r="F17" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
-      </c>
-      <c r="G18" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    Bedclock_IDF_V07 : Test FreeRTOS</v>
-      </c>
-      <c r="N18" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  * `Bedclock_IDF_V07` : Test FreeRTOS</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
-      </c>
-      <c r="G19" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    Bedclock_IDF_V08 : Implement multiple parallel processes</v>
-      </c>
-      <c r="N19" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  * `Bedclock_IDF_V08` : Implement multiple parallel processes</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    Bedclock_IDF_V09 : Internal Espressif SSD1306 driver including LVGL</v>
-      </c>
-      <c r="N20" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  * `Bedclock_IDF_V09` : Internal Espressif SSD1306 driver including LVGL</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>0</v>
       </c>
       <c r="B21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
         <v>6</v>
-      </c>
-      <c r="G21" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    Bedclock_IDF_V10 : First working version of application</v>
-      </c>
-      <c r="N21" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  * `Bedclock_IDF_V10` : First working version of application</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G22" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve">    Bedclock_IDF_V11 : First working version of pixel buffer</v>
-      </c>
-      <c r="N22" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  * `Bedclock_IDF_V11` : First working version of pixel buffer</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G23" t="str">
-        <f>"    "&amp;C15&amp;" : "&amp;B15</f>
-        <v xml:space="preserve">    Bedclock_IDF_V12 : Scrolling example LVGL</v>
-      </c>
-      <c r="N23" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve">  * `Bedclock_IDF_V12` : Scrolling example LVGL</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="G24" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2690,7 +2657,7 @@
         <v xml:space="preserve">0.03, </v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H1" t="str">
         <f>A1&amp;"      "&amp;F1</f>
@@ -2707,7 +2674,7 @@
         <v xml:space="preserve">0.06, </v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H2" t="str">
         <f>A2&amp;"      "&amp;F2</f>
@@ -2720,7 +2687,7 @@
         <v xml:space="preserve">0.16, </v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="H3" t="str">
         <f>A3&amp;"      "&amp;F3</f>
@@ -2733,7 +2700,7 @@
         <v xml:space="preserve">0.40, </v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="H4" t="str">
         <f>A4&amp;"      "&amp;F4</f>
@@ -2746,7 +2713,7 @@
         <v xml:space="preserve">1.00, </v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H5" t="str">
         <f>A5&amp;"      "&amp;F5</f>
@@ -2762,7 +2729,7 @@
         <v xml:space="preserve">5*60*1000, </v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D7" t="str">
         <f t="shared" ref="D7:D11" si="0">A7&amp;"      "&amp;B7</f>
@@ -2781,7 +2748,7 @@
         <v xml:space="preserve">7*60*1000, </v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D8" t="str">
         <f t="shared" si="0"/>
@@ -2798,7 +2765,7 @@
         <v xml:space="preserve">10*60*1000, </v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
@@ -2815,7 +2782,7 @@
         <v xml:space="preserve">14*60*1000, </v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -2832,7 +2799,7 @@
         <v xml:space="preserve">20*60*1000, </v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -2845,25 +2812,25 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="D13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F13" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="L13" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="M13" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="N13" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
@@ -2880,7 +2847,7 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F14" t="str">
         <f>"  { .r = "&amp;TEXT(B14,"0.000")&amp;",  .g = "&amp;TEXT(C14,"0.000")&amp;",  .b = "&amp;TEXT(D14,"0.000")&amp;" },    // "&amp;TEXT(A14,"0")&amp;" = "&amp;E14</f>
@@ -2922,7 +2889,7 @@
         <v>0.67026194144838214</v>
       </c>
       <c r="E15" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F15" t="str">
         <f>"  { .r = "&amp;TEXT(B15,"0.000")&amp;",  .g = "&amp;TEXT(C15,"0.000")&amp;",  .b = "&amp;TEXT(D15,"0.000")&amp;" },    // "&amp;TEXT(A15,"0")&amp;" = "&amp;E15</f>
@@ -2966,7 +2933,7 @@
         <v>0.72864321608040206</v>
       </c>
       <c r="E16" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F16" t="str">
         <f>"  { .r = "&amp;TEXT(B16,"0.000")&amp;",  .g = "&amp;TEXT(C16,"0.000")&amp;",  .b = "&amp;TEXT(D16,"0.000")&amp;" },    // "&amp;TEXT(A16,"0")&amp;" = "&amp;E16</f>
@@ -3008,7 +2975,7 @@
         <v>0.75</v>
       </c>
       <c r="E17" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F17" t="str">
         <f>"  { .r = "&amp;TEXT(B17,"0.000")&amp;",  .g = "&amp;TEXT(C17,"0.000")&amp;",  .b = "&amp;TEXT(D17,"0.000")&amp;" },    // "&amp;TEXT(A17,"0")&amp;" = "&amp;E17</f>
@@ -3038,7 +3005,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="F18" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.45">
@@ -3062,7 +3029,7 @@
         <v>2.5148667298248704</v>
       </c>
       <c r="F20" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="L20">
         <f>L19/$O$19</f>
@@ -3143,12 +3110,12 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.45">
       <c r="F26" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B28">
         <v>40</v>
@@ -3156,7 +3123,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -3168,7 +3135,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -3176,7 +3143,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B34">
         <v>20</v>
@@ -3184,15 +3151,15 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C35" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D35" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B36" s="12">
         <f>LOOKUP($B$32,$A$14:$A$17,B14:B17)</f>
@@ -3209,7 +3176,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B37" s="12">
         <f>LOOKUP($B$32,$A$14:$A$17,C14:C17)</f>
@@ -3226,7 +3193,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B38" s="12">
         <f>LOOKUP($B$32,$A$14:$A$17,D14:D17)</f>
@@ -3723,7 +3690,7 @@
         <v>15.967105496833609</v>
       </c>
       <c r="F64" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
@@ -3778,7 +3745,7 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="F68" s="4" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3807,7 +3774,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B1">
         <v>16</v>
@@ -3815,13 +3782,13 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.45">
@@ -3835,7 +3802,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
@@ -3849,7 +3816,7 @@
         <v>-32</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.45">
@@ -3863,7 +3830,7 @@
         <v>-56</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.45">
@@ -3880,7 +3847,7 @@
         <v>-72</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.45">
@@ -3897,7 +3864,7 @@
         <v>-88</v>
       </c>
       <c r="D8" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.45">
@@ -3914,7 +3881,7 @@
         <v>-104</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
@@ -4037,7 +4004,7 @@
         <v>5120</v>
       </c>
       <c r="M17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.45">
@@ -4046,69 +4013,69 @@
         <v>640</v>
       </c>
       <c r="M18" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B20">
         <v>128</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B21">
         <v>32</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B22">
         <f>B20*B21</f>
         <v>4096</v>
       </c>
       <c r="C22" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B23">
         <f>B22/8</f>
         <v>512</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B25">
         <v>400000</v>
       </c>
       <c r="C25" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B26" s="10">
         <v>0.8</v>
@@ -4116,14 +4083,14 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B27">
         <f>B22/(B25*B26)</f>
         <v>1.2800000000000001E-2</v>
       </c>
       <c r="C27" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.45">
@@ -4132,7 +4099,7 @@
         <v>12.8</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -4154,7 +4121,7 @@
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.45">
       <c r="D2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.45">
@@ -4224,7 +4191,7 @@
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
@@ -4820,22 +4787,22 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.45">
       <c r="C1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="O1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="P1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="Q1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="S1">
         <v>671</v>
@@ -4861,18 +4828,18 @@
         <v>671</v>
       </c>
       <c r="AA1" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="AB1" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="AC1" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <f>SEARCH(C$1,$A2)</f>
@@ -4961,7 +4928,7 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C39" si="5">SEARCH(C$1,$A3)</f>
@@ -5050,7 +5017,7 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <f t="shared" si="5"/>
@@ -5139,7 +5106,7 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <f t="shared" si="5"/>
@@ -5216,7 +5183,7 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <f t="shared" si="5"/>
@@ -5297,7 +5264,7 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C7">
         <f t="shared" si="5"/>
@@ -5378,7 +5345,7 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <f t="shared" si="5"/>
@@ -5459,7 +5426,7 @@
     </row>
     <row r="9" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <f t="shared" si="5"/>
@@ -5536,7 +5503,7 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C10">
         <f t="shared" si="5"/>
@@ -5613,7 +5580,7 @@
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C11">
         <f t="shared" si="5"/>
@@ -5690,7 +5657,7 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <f t="shared" si="5"/>
@@ -5767,7 +5734,7 @@
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C13">
         <f t="shared" si="5"/>
@@ -5844,7 +5811,7 @@
     </row>
     <row r="14" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C14">
         <f t="shared" si="5"/>
@@ -5921,7 +5888,7 @@
     </row>
     <row r="15" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C15">
         <f t="shared" si="5"/>
@@ -5998,7 +5965,7 @@
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C16">
         <f t="shared" si="5"/>
@@ -6075,7 +6042,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C17">
         <f t="shared" si="5"/>
@@ -6152,7 +6119,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C18">
         <f t="shared" si="5"/>
@@ -6229,7 +6196,7 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C19">
         <f t="shared" si="5"/>
@@ -6306,7 +6273,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C20">
         <f t="shared" si="5"/>
@@ -6383,7 +6350,7 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C21">
         <f t="shared" si="5"/>
@@ -6460,7 +6427,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C22">
         <f t="shared" si="5"/>
@@ -6537,7 +6504,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C23">
         <f t="shared" si="5"/>
@@ -6614,7 +6581,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C24">
         <f t="shared" si="5"/>
@@ -6691,7 +6658,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C25">
         <f t="shared" si="5"/>
@@ -6768,7 +6735,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C26">
         <f t="shared" si="5"/>
@@ -6845,7 +6812,7 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C27">
         <f t="shared" si="5"/>
@@ -6922,7 +6889,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C28">
         <f t="shared" si="5"/>
@@ -6999,7 +6966,7 @@
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C29">
         <f t="shared" si="5"/>
@@ -7076,7 +7043,7 @@
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C30">
         <f t="shared" si="5"/>
@@ -7153,7 +7120,7 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C31">
         <f t="shared" si="5"/>
@@ -7230,7 +7197,7 @@
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C32">
         <f t="shared" si="5"/>
@@ -7307,7 +7274,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C33">
         <f t="shared" si="5"/>
@@ -7384,7 +7351,7 @@
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C34">
         <f t="shared" si="5"/>
@@ -7461,7 +7428,7 @@
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C35">
         <f t="shared" si="5"/>
@@ -7538,7 +7505,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C36">
         <f t="shared" si="5"/>
@@ -7615,7 +7582,7 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C37">
         <f t="shared" si="5"/>
@@ -7692,7 +7659,7 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C38">
         <f t="shared" si="5"/>
@@ -7769,7 +7736,7 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C39">
         <f t="shared" si="5"/>
@@ -8688,42 +8655,42 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="D3">
         <f>HEX2DEC(C3)</f>
         <v>36864</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="G3">
         <f>HEX2DEC(F3)</f>
@@ -8732,17 +8699,17 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D4">
         <f>HEX2DEC(C4)</f>
         <v>57344</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G4">
         <f>HEX2DEC(F4)</f>
@@ -8751,17 +8718,17 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D5">
         <f>HEX2DEC(C5)</f>
         <v>65536</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G5">
         <f>HEX2DEC(F5)</f>
@@ -8770,17 +8737,17 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D6">
         <f>HEX2DEC(C6)</f>
         <v>4128768</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G6">
         <f>HEX2DEC(F6)</f>

</xml_diff>

<commit_message>
Mapped LED colors on color temperature
</commit_message>
<xml_diff>
--- a/04_Software/Porting to ESP-IDF.xlsx
+++ b/04_Software/Porting to ESP-IDF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\henkj\Documents\GitHub\BedClock\04_Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50725FD1-EAE4-4909-BD42-631CDF249114}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D3F85A8-8211-408F-93AC-77B74AA6EDA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{877FF0B8-2AAA-4A03-B534-DDBA6ED9C717}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{877FF0B8-2AAA-4A03-B534-DDBA6ED9C717}"/>
   </bookViews>
   <sheets>
     <sheet name="progress" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="152">
   <si>
     <t>Test WS2812 led chain</t>
   </si>
@@ -424,15 +424,6 @@
     <t xml:space="preserve">const led_color_t LED_COLORS[] = { </t>
   </si>
   <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>Yellow</t>
-  </si>
-  <si>
-    <t>Orange</t>
-  </si>
-  <si>
     <t>Red</t>
   </si>
   <si>
@@ -506,14 +497,28 @@
   </si>
   <si>
     <t>"| Directory | Purpose |</t>
+  </si>
+  <si>
+    <t>R%</t>
+  </si>
+  <si>
+    <t>G%</t>
+  </si>
+  <si>
+    <t>B%</t>
+  </si>
+  <si>
+    <t>Temp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="General&quot; K&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -584,7 +589,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -604,6 +609,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2306,9 +2313,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E3FDF8-1B80-46E7-8A6B-8969C0129D64}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2343,21 +2350,21 @@
     <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
       <c r="F3" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="F4" t="s">
+        <v>142</v>
+      </c>
+      <c r="G4" t="s">
         <v>145</v>
       </c>
-      <c r="G4" t="s">
-        <v>148</v>
-      </c>
       <c r="H4" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
@@ -2577,7 +2584,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C14" t="s">
         <v>82</v>
@@ -2600,7 +2607,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s">
         <v>94</v>
@@ -2623,10 +2630,10 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C16" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
@@ -2649,7 +2656,7 @@
         <v>108</v>
       </c>
       <c r="F17" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -2700,10 +2707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6F3A0C-BCE4-45A2-918D-4AA29D9B0FCD}">
-  <dimension ref="A1:R68"/>
+  <dimension ref="A1:R72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:F18"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2801,6 +2808,10 @@
       <c r="G7">
         <v>1.4142136085596386</v>
       </c>
+      <c r="I7" t="str">
+        <f>TEXT(F7,"0")&amp;" min"</f>
+        <v>5 min</v>
+      </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="str">
@@ -2818,6 +2829,10 @@
         <f>F7*$G$7</f>
         <v>7.0710680427981929</v>
       </c>
+      <c r="I8" t="str">
+        <f>I7&amp;", "&amp;TEXT(F8,"0")&amp;" min"</f>
+        <v>5 min, 7 min</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="str">
@@ -2835,6 +2850,10 @@
         <f t="shared" ref="F9:F11" si="1">F8*$G$7</f>
         <v>10.000000653176373</v>
       </c>
+      <c r="I9" t="str">
+        <f>I8&amp;", "&amp;TEXT(F9,"0")&amp;" min"</f>
+        <v>5 min, 7 min, 10 min</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="str">
@@ -2852,6 +2871,10 @@
         <f t="shared" si="1"/>
         <v>14.142137009327302</v>
       </c>
+      <c r="I10" t="str">
+        <f>I9&amp;", "&amp;TEXT(F10,"0")&amp;" min"</f>
+        <v>5 min, 7 min, 10 min, 14 min</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="str">
@@ -2869,28 +2892,44 @@
         <f t="shared" si="1"/>
         <v>20.000002612705579</v>
       </c>
+      <c r="I11" t="str">
+        <f>I10&amp;", "&amp;TEXT(F11,"0")&amp;" min"</f>
+        <v>5 min, 7 min, 10 min, 14 min, 20 min</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F13" t="s">
         <v>122</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L13" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="M13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="M13" t="s">
-        <v>136</v>
-      </c>
-      <c r="N13" t="s">
-        <v>137</v>
+      <c r="N13" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="R13" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.45">
@@ -2898,41 +2937,47 @@
         <v>0</v>
       </c>
       <c r="B14" s="11">
-        <v>1</v>
+        <f>LOOKUP($E14,$L$14:$L$20,P$14:P$20)</f>
+        <v>1.0079051383399209</v>
       </c>
       <c r="C14" s="11">
-        <v>1</v>
+        <f t="shared" ref="C14:C17" si="2">LOOKUP($E14,$L$14:$L$20,Q$14:Q$20)</f>
+        <v>1.0039525691699605</v>
       </c>
       <c r="D14" s="11">
-        <v>1</v>
-      </c>
-      <c r="E14" t="s">
-        <v>123</v>
+        <f t="shared" ref="D14:D17" si="3">LOOKUP($E14,$L$14:$L$20,R$14:R$20)</f>
+        <v>0.98814229249011865</v>
+      </c>
+      <c r="E14">
+        <v>6500</v>
       </c>
       <c r="F14" t="str">
-        <f>"  { .r = "&amp;TEXT(B14,"0.000")&amp;",  .g = "&amp;TEXT(C14,"0.000")&amp;",  .b = "&amp;TEXT(D14,"0.000")&amp;" },    // "&amp;TEXT(A14,"0")&amp;" = "&amp;E14</f>
-        <v xml:space="preserve">  { .r = 1.000,  .g = 1.000,  .b = 1.000 },    // 0 = White</v>
-      </c>
-      <c r="L14">
-        <v>1</v>
+        <f>"  { .r = "&amp;TEXT(B14,"0.000")&amp;",  .g = "&amp;TEXT(C14,"0.000")&amp;",  .b = "&amp;TEXT(D14,"0.000")&amp;" },    // "&amp;TEXT(A14,"0")&amp;" = "&amp;E14&amp;" K"</f>
+        <v xml:space="preserve">  { .r = 1.008,  .g = 1.004,  .b = 0.988 },    // 0 = 6500 K</v>
+      </c>
+      <c r="L14" s="15">
+        <v>3000</v>
       </c>
       <c r="M14">
-        <v>1</v>
+        <v>255</v>
       </c>
       <c r="N14">
-        <v>1</v>
+        <v>177</v>
+      </c>
+      <c r="O14">
+        <v>110</v>
       </c>
       <c r="P14">
-        <f t="shared" ref="P14:R17" si="2">L14/AVERAGE($L14:$N14)</f>
-        <v>1</v>
+        <f>M14/SUM($M14:$O14)*3</f>
+        <v>1.411439114391144</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>N14/SUM($M14:$O14)*3</f>
+        <v>0.97970479704797053</v>
       </c>
       <c r="R14">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>O14/SUM($M14:$O14)*3</f>
+        <v>0.60885608856088558</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.45">
@@ -2940,43 +2985,47 @@
         <v>1</v>
       </c>
       <c r="B15" s="11">
-        <v>1.1787365177195686</v>
+        <f t="shared" ref="B15:B17" si="4">LOOKUP($E15,$L$14:$L$20,P$14:P$20)</f>
+        <v>1.1103047895500726</v>
       </c>
       <c r="C15" s="11">
-        <v>1.1510015408320493</v>
+        <f t="shared" si="2"/>
+        <v>0.99274310595065318</v>
       </c>
       <c r="D15" s="11">
-        <v>0.67026194144838214</v>
-      </c>
-      <c r="E15" t="s">
-        <v>124</v>
+        <f t="shared" si="3"/>
+        <v>0.89695210449927432</v>
+      </c>
+      <c r="E15">
+        <v>5000</v>
       </c>
       <c r="F15" t="str">
-        <f>"  { .r = "&amp;TEXT(B15,"0.000")&amp;",  .g = "&amp;TEXT(C15,"0.000")&amp;",  .b = "&amp;TEXT(D15,"0.000")&amp;" },    // "&amp;TEXT(A15,"0")&amp;" = "&amp;E15</f>
-        <v xml:space="preserve">  { .r = 1.179,  .g = 1.151,  .b = 0.670 },    // 1 = Yellow</v>
-      </c>
-      <c r="L15">
-        <v>1</v>
+        <f t="shared" ref="F15:F17" si="5">"  { .r = "&amp;TEXT(B15,"0.000")&amp;",  .g = "&amp;TEXT(C15,"0.000")&amp;",  .b = "&amp;TEXT(D15,"0.000")&amp;" },    // "&amp;TEXT(A15,"0")&amp;" = "&amp;E15&amp;" K"</f>
+        <v xml:space="preserve">  { .r = 1.110,  .g = 0.993,  .b = 0.897 },    // 1 = 5000 K</v>
+      </c>
+      <c r="L15" s="15">
+        <v>4000</v>
       </c>
       <c r="M15">
-        <f>249/255</f>
-        <v>0.97647058823529409</v>
+        <v>255</v>
       </c>
       <c r="N15">
-        <f>145/255</f>
-        <v>0.56862745098039214</v>
+        <v>206</v>
+      </c>
+      <c r="O15">
+        <v>166</v>
       </c>
       <c r="P15">
-        <f t="shared" si="2"/>
-        <v>1.1787365177195686</v>
+        <f>M15/SUM($M15:$O15)*3</f>
+        <v>1.2200956937799043</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="2"/>
-        <v>1.1510015408320493</v>
+        <f>N15/SUM($M15:$O15)*3</f>
+        <v>0.9856459330143541</v>
       </c>
       <c r="R15">
-        <f t="shared" si="2"/>
-        <v>0.67026194144838214</v>
+        <f>O15/SUM($M15:$O15)*3</f>
+        <v>0.79425837320574155</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.45">
@@ -2984,41 +3033,47 @@
         <v>2</v>
       </c>
       <c r="B16" s="11">
-        <v>1.2814070351758795</v>
+        <f t="shared" si="4"/>
+        <v>1.2200956937799043</v>
       </c>
       <c r="C16" s="11">
-        <v>0.98994974874371855</v>
+        <f t="shared" si="2"/>
+        <v>0.9856459330143541</v>
       </c>
       <c r="D16" s="11">
-        <v>0.72864321608040206</v>
-      </c>
-      <c r="E16" t="s">
-        <v>125</v>
+        <f t="shared" si="3"/>
+        <v>0.79425837320574155</v>
+      </c>
+      <c r="E16">
+        <v>4000</v>
       </c>
       <c r="F16" t="str">
-        <f>"  { .r = "&amp;TEXT(B16,"0.000")&amp;",  .g = "&amp;TEXT(C16,"0.000")&amp;",  .b = "&amp;TEXT(D16,"0.000")&amp;" },    // "&amp;TEXT(A16,"0")&amp;" = "&amp;E16</f>
-        <v xml:space="preserve">  { .r = 1.281,  .g = 0.990,  .b = 0.729 },    // 2 = Orange</v>
-      </c>
-      <c r="L16">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  { .r = 1.220,  .g = 0.986,  .b = 0.794 },    // 2 = 4000 K</v>
+      </c>
+      <c r="L16" s="15">
+        <v>5000</v>
+      </c>
+      <c r="M16">
         <v>255</v>
       </c>
-      <c r="M16">
-        <v>197</v>
-      </c>
       <c r="N16">
-        <v>145</v>
+        <v>228</v>
+      </c>
+      <c r="O16">
+        <v>206</v>
       </c>
       <c r="P16">
-        <f t="shared" si="2"/>
-        <v>1.2814070351758795</v>
+        <f>M16/SUM($M16:$O16)*3</f>
+        <v>1.1103047895500726</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="2"/>
-        <v>0.98994974874371855</v>
+        <f>N16/SUM($M16:$O16)*3</f>
+        <v>0.99274310595065318</v>
       </c>
       <c r="R16">
-        <f t="shared" si="2"/>
-        <v>0.72864321608040206</v>
+        <f>O16/SUM($M16:$O16)*3</f>
+        <v>0.89695210449927432</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.45">
@@ -3026,62 +3081,102 @@
         <v>3</v>
       </c>
       <c r="B17" s="11">
-        <v>1.5</v>
+        <f t="shared" si="4"/>
+        <v>1.411439114391144</v>
       </c>
       <c r="C17" s="11">
-        <v>0.75</v>
+        <f t="shared" si="2"/>
+        <v>0.97970479704797053</v>
       </c>
       <c r="D17" s="11">
-        <v>0.75</v>
-      </c>
-      <c r="E17" t="s">
-        <v>126</v>
+        <f t="shared" si="3"/>
+        <v>0.60885608856088558</v>
+      </c>
+      <c r="E17">
+        <v>3000</v>
       </c>
       <c r="F17" t="str">
-        <f>"  { .r = "&amp;TEXT(B17,"0.000")&amp;",  .g = "&amp;TEXT(C17,"0.000")&amp;",  .b = "&amp;TEXT(D17,"0.000")&amp;" },    // "&amp;TEXT(A17,"0")&amp;" = "&amp;E17</f>
-        <v xml:space="preserve">  { .r = 1.500,  .g = 0.750,  .b = 0.750 },    // 3 = Red</v>
-      </c>
-      <c r="L17">
+        <f t="shared" si="5"/>
+        <v xml:space="preserve">  { .r = 1.411,  .g = 0.980,  .b = 0.609 },    // 3 = 3000 K</v>
+      </c>
+      <c r="L17" s="15">
+        <v>5500</v>
+      </c>
+      <c r="M17">
         <v>255</v>
       </c>
-      <c r="M17">
-        <v>85</v>
-      </c>
       <c r="N17">
-        <v>85</v>
+        <v>237</v>
+      </c>
+      <c r="O17">
+        <v>222</v>
       </c>
       <c r="P17">
-        <f t="shared" si="2"/>
-        <v>1.8</v>
+        <f>M17/SUM($M17:$O17)*3</f>
+        <v>1.0714285714285714</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="2"/>
-        <v>0.60000000000000009</v>
+        <f>N17/SUM($M17:$O17)*3</f>
+        <v>0.99579831932773111</v>
       </c>
       <c r="R17">
-        <f t="shared" si="2"/>
-        <v>0.60000000000000009</v>
+        <f>O17/SUM($M17:$O17)*3</f>
+        <v>0.9327731092436975</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.45">
       <c r="F18" t="s">
         <v>121</v>
       </c>
+      <c r="L18" s="15">
+        <v>6000</v>
+      </c>
+      <c r="M18">
+        <v>255</v>
+      </c>
+      <c r="N18">
+        <v>246</v>
+      </c>
+      <c r="O18">
+        <v>237</v>
+      </c>
+      <c r="P18">
+        <f>M18/SUM($M18:$O18)*3</f>
+        <v>1.0365853658536586</v>
+      </c>
+      <c r="Q18">
+        <f>N18/SUM($M18:$O18)*3</f>
+        <v>1</v>
+      </c>
+      <c r="R18">
+        <f>O18/SUM($M18:$O18)*3</f>
+        <v>0.96341463414634154</v>
+      </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="L19">
-        <v>1.5</v>
+      <c r="L19" s="15">
+        <v>6200</v>
       </c>
       <c r="M19">
-        <v>0.75</v>
+        <v>255</v>
       </c>
       <c r="N19">
-        <f>M19</f>
-        <v>0.75</v>
+        <v>249</v>
       </c>
       <c r="O19">
-        <f>AVERAGE(L19:N19)</f>
-        <v>1</v>
+        <v>242</v>
+      </c>
+      <c r="P19">
+        <f>M19/SUM($M19:$O19)*3</f>
+        <v>1.0254691689008042</v>
+      </c>
+      <c r="Q19">
+        <f>N19/SUM($M19:$O19)*3</f>
+        <v>1.0013404825737267</v>
+      </c>
+      <c r="R19">
+        <f>O19/SUM($M19:$O19)*3</f>
+        <v>0.97319034852546915</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.45">
@@ -3089,19 +3184,31 @@
         <v>2.5148667298248704</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
-      </c>
-      <c r="L20">
-        <f>L19/$O$19</f>
-        <v>1.5</v>
+        <v>125</v>
+      </c>
+      <c r="L20" s="15">
+        <v>6500</v>
       </c>
       <c r="M20">
-        <f>M19/$O$19</f>
-        <v>0.75</v>
+        <v>255</v>
       </c>
       <c r="N20">
-        <f>N19/$O$19</f>
-        <v>0.75</v>
+        <v>254</v>
+      </c>
+      <c r="O20">
+        <v>250</v>
+      </c>
+      <c r="P20">
+        <f>M20/SUM($M20:$O20)*3</f>
+        <v>1.0079051383399209</v>
+      </c>
+      <c r="Q20">
+        <f>N20/SUM($M20:$O20)*3</f>
+        <v>1.0039525691699605</v>
+      </c>
+      <c r="R20">
+        <f>O20/SUM($M20:$O20)*3</f>
+        <v>0.98814229249011865</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.45">
@@ -3115,6 +3222,10 @@
         <f>"    "&amp;TEXT(B21,"0.000")&amp;",  // .led_intensity = "&amp;TEXT(A21,"0")</f>
         <v xml:space="preserve">    0.025,  // .led_intensity = 0</v>
       </c>
+      <c r="J21" t="str">
+        <f>TEXT(100*B21,"0.0")&amp;"%"</f>
+        <v>2.5%</v>
+      </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A22">
@@ -3125,8 +3236,16 @@
         <v>6.2871668245621765E-2</v>
       </c>
       <c r="F22" t="str">
-        <f t="shared" ref="F22:F25" si="3">"    "&amp;TEXT(B22,"0.000")&amp;",  // .led_intensity = "&amp;TEXT(A22,"0")</f>
+        <f t="shared" ref="F22:F25" si="6">"    "&amp;TEXT(B22,"0.000")&amp;",  // .led_intensity = "&amp;TEXT(A22,"0")</f>
         <v xml:space="preserve">    0.063,  // .led_intensity = 1</v>
+      </c>
+      <c r="J22" t="str">
+        <f>J21&amp;", "&amp;TEXT(100*B22,"0")&amp;"%"</f>
+        <v>2.5%, 6%</v>
+      </c>
+      <c r="N22" t="str">
+        <f>E14&amp;" K"</f>
+        <v>6500 K</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.45">
@@ -3138,8 +3257,16 @@
         <v>0.15811386671950095</v>
       </c>
       <c r="F23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">    0.158,  // .led_intensity = 2</v>
+      </c>
+      <c r="J23" t="str">
+        <f>J22&amp;", "&amp;TEXT(100*B23,"0")&amp;"%"</f>
+        <v>2.5%, 6%, 16%</v>
+      </c>
+      <c r="N23" t="str">
+        <f>N22&amp;", "&amp;TEXT(E15,"0")&amp;" K"</f>
+        <v>6500 K, 5000 K</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.45">
@@ -3151,8 +3278,16 @@
         <v>0.39763530293683674</v>
       </c>
       <c r="F24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">    0.398,  // .led_intensity = 3</v>
+      </c>
+      <c r="J24" t="str">
+        <f>J23&amp;", "&amp;TEXT(100*B24,"0")&amp;"%"</f>
+        <v>2.5%, 6%, 16%, 40%</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" ref="N24:N25" si="7">N23&amp;", "&amp;TEXT(E16,"0")&amp;" K"</f>
+        <v>6500 K, 5000 K, 4000 K</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.45">
@@ -3164,8 +3299,16 @@
         <v>0.9999997939596843</v>
       </c>
       <c r="F25" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v xml:space="preserve">    1.000,  // .led_intensity = 4</v>
+      </c>
+      <c r="J25" t="str">
+        <f>J24&amp;", "&amp;TEXT(100*B25,"0")&amp;"%"</f>
+        <v>2.5%, 6%, 16%, 40%, 100%</v>
+      </c>
+      <c r="N25" t="str">
+        <f t="shared" si="7"/>
+        <v>6500 K, 5000 K, 4000 K, 3000 K</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.45">
@@ -3175,7 +3318,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B28">
         <v>40</v>
@@ -3183,7 +3326,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B30">
         <v>2</v>
@@ -3195,7 +3338,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B32">
         <v>2</v>
@@ -3203,7 +3346,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B34">
         <v>20</v>
@@ -3211,61 +3354,61 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="C35" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D35" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B36" s="12">
         <f>LOOKUP($B$32,$A$14:$A$17,B14:B17)</f>
-        <v>1.2814070351758795</v>
+        <v>1.2200956937799043</v>
       </c>
       <c r="C36" s="12">
         <f>$B$28*$C$30*B36</f>
-        <v>8.1043288469291959</v>
+        <v>7.7165619164541139</v>
       </c>
       <c r="D36" s="12">
         <f>C36/$B$34</f>
-        <v>0.40521644234645982</v>
+        <v>0.38582809582270572</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B37" s="12">
         <f>LOOKUP($B$32,$A$14:$A$17,C14:C17)</f>
-        <v>0.98994974874371855</v>
+        <v>0.9856459330143541</v>
       </c>
       <c r="C37" s="12">
         <f>$B$28*$C$30*B37</f>
-        <v>6.260991305274711</v>
+        <v>6.2337715874099899</v>
       </c>
       <c r="D37" s="12">
         <f>C37/$B$34</f>
-        <v>0.31304956526373556</v>
+        <v>0.31168857937049949</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B38" s="12">
         <f>LOOKUP($B$32,$A$14:$A$17,D14:D17)</f>
-        <v>0.72864321608040206</v>
+        <v>0.79425837320574155</v>
       </c>
       <c r="C38" s="12">
         <f>$B$28*$C$30*B38</f>
-        <v>4.6083438541362094</v>
+        <v>5.0233305024760107</v>
       </c>
       <c r="D38" s="12">
         <f>C38/$B$34</f>
-        <v>0.23041719270681046</v>
+        <v>0.25116652512380055</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
@@ -3286,19 +3429,19 @@
     <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" t="str">
         <f>A41&amp;", "&amp;TEXT(B42,"0.00")</f>
-        <v>0.00, 0.41</v>
+        <v>0.00, 0.39</v>
       </c>
       <c r="B42" s="12">
         <f>B41+$D$36</f>
-        <v>0.40521644234645982</v>
+        <v>0.38582809582270572</v>
       </c>
       <c r="C42" s="12">
         <f>C41+$D$37</f>
-        <v>0.31304956526373556</v>
+        <v>0.31168857937049949</v>
       </c>
       <c r="D42" s="12">
         <f>D41+$D$38</f>
-        <v>0.23041719270681046</v>
+        <v>0.25116652512380055</v>
       </c>
       <c r="F42" s="13">
         <f>INT(B42)</f>
@@ -3315,428 +3458,428 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="str">
-        <f t="shared" ref="A43:A52" si="4">A42&amp;", "&amp;TEXT(B43,"0.00")</f>
-        <v>0.00, 0.41, 0.81</v>
+        <f t="shared" ref="A43:A52" si="8">A42&amp;", "&amp;TEXT(B43,"0.00")</f>
+        <v>0.00, 0.39, 0.77</v>
       </c>
       <c r="B43" s="12">
-        <f t="shared" ref="B43:B60" si="5">B42+$D$36</f>
-        <v>0.81043288469291963</v>
+        <f t="shared" ref="B43:B60" si="9">B42+$D$36</f>
+        <v>0.77165619164541144</v>
       </c>
       <c r="C43" s="12">
-        <f t="shared" ref="C43:C60" si="6">C42+$D$37</f>
-        <v>0.62609913052747113</v>
+        <f t="shared" ref="C43:C60" si="10">C42+$D$37</f>
+        <v>0.62337715874099897</v>
       </c>
       <c r="D43" s="12">
-        <f t="shared" ref="D43:D60" si="7">D42+$D$38</f>
-        <v>0.46083438541362093</v>
+        <f t="shared" ref="D43:D60" si="11">D42+$D$38</f>
+        <v>0.50233305024760111</v>
       </c>
       <c r="F43" s="13">
-        <f t="shared" ref="F43:F52" si="8">INT(B43)</f>
+        <f t="shared" ref="F43:F52" si="12">INT(B43)</f>
         <v>0</v>
       </c>
       <c r="G43">
-        <f t="shared" ref="G43:G52" si="9">INT(16*MOD(B43,1))</f>
+        <f t="shared" ref="G43:G52" si="13">INT(16*MOD(B43,1))</f>
         <v>12</v>
       </c>
       <c r="I43">
-        <f t="shared" ref="I43:I52" si="10">F43+G43/16</f>
+        <f t="shared" ref="I43:I52" si="14">F43+G43/16</f>
         <v>0.75</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" t="str">
-        <f t="shared" si="4"/>
-        <v>0.00, 0.41, 0.81, 1.22</v>
+        <f t="shared" si="8"/>
+        <v>0.00, 0.39, 0.77, 1.16</v>
       </c>
       <c r="B44" s="12">
-        <f t="shared" si="5"/>
-        <v>1.2156493270393796</v>
+        <f t="shared" si="9"/>
+        <v>1.157484287468117</v>
       </c>
       <c r="C44" s="12">
-        <f t="shared" si="6"/>
-        <v>0.93914869579120674</v>
+        <f t="shared" si="10"/>
+        <v>0.9350657381114984</v>
       </c>
       <c r="D44" s="12">
-        <f t="shared" si="7"/>
-        <v>0.69125157812043136</v>
+        <f t="shared" si="11"/>
+        <v>0.75349957537140166</v>
       </c>
       <c r="F44" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G44">
-        <f t="shared" si="9"/>
-        <v>3</v>
+        <f t="shared" si="13"/>
+        <v>2</v>
       </c>
       <c r="I44">
-        <f t="shared" si="10"/>
-        <v>1.1875</v>
+        <f t="shared" si="14"/>
+        <v>1.125</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" t="str">
-        <f t="shared" si="4"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62</v>
+        <f t="shared" si="8"/>
+        <v>0.00, 0.39, 0.77, 1.16, 1.54</v>
       </c>
       <c r="B45" s="12">
-        <f t="shared" si="5"/>
-        <v>1.6208657693858393</v>
+        <f t="shared" si="9"/>
+        <v>1.5433123832908229</v>
       </c>
       <c r="C45" s="12">
-        <f t="shared" si="6"/>
-        <v>1.2521982610549423</v>
+        <f t="shared" si="10"/>
+        <v>1.2467543174819979</v>
       </c>
       <c r="D45" s="12">
-        <f t="shared" si="7"/>
-        <v>0.92166877082724186</v>
+        <f t="shared" si="11"/>
+        <v>1.0046661004952022</v>
       </c>
       <c r="F45" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G45">
-        <f t="shared" si="9"/>
-        <v>9</v>
+        <f t="shared" si="13"/>
+        <v>8</v>
       </c>
       <c r="I45">
-        <f t="shared" si="10"/>
-        <v>1.5625</v>
+        <f t="shared" si="14"/>
+        <v>1.5</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" t="str">
-        <f t="shared" si="4"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03</v>
+        <f t="shared" si="8"/>
+        <v>0.00, 0.39, 0.77, 1.16, 1.54, 1.93</v>
       </c>
       <c r="B46" s="12">
-        <f t="shared" si="5"/>
-        <v>2.026082211732299</v>
+        <f t="shared" si="9"/>
+        <v>1.9291404791135287</v>
       </c>
       <c r="C46" s="12">
-        <f t="shared" si="6"/>
-        <v>1.5652478263186778</v>
+        <f t="shared" si="10"/>
+        <v>1.5584428968524975</v>
       </c>
       <c r="D46" s="12">
-        <f t="shared" si="7"/>
-        <v>1.1520859635340523</v>
+        <f t="shared" si="11"/>
+        <v>1.2558326256190027</v>
       </c>
       <c r="F46" s="13">
-        <f t="shared" si="8"/>
-        <v>2</v>
+        <f t="shared" si="12"/>
+        <v>1</v>
       </c>
       <c r="G46">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>14</v>
       </c>
       <c r="I46">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f t="shared" si="14"/>
+        <v>1.875</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" t="str">
-        <f t="shared" si="4"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43</v>
+        <f t="shared" si="8"/>
+        <v>0.00, 0.39, 0.77, 1.16, 1.54, 1.93, 2.31</v>
       </c>
       <c r="B47" s="12">
-        <f t="shared" si="5"/>
-        <v>2.4312986540787587</v>
+        <f t="shared" si="9"/>
+        <v>2.3149685749362345</v>
       </c>
       <c r="C47" s="12">
-        <f t="shared" si="6"/>
-        <v>1.8782973915824133</v>
+        <f t="shared" si="10"/>
+        <v>1.870131476222997</v>
       </c>
       <c r="D47" s="12">
-        <f t="shared" si="7"/>
-        <v>1.3825031562408627</v>
+        <f t="shared" si="11"/>
+        <v>1.5069991507428031</v>
       </c>
       <c r="F47" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="G47">
-        <f t="shared" si="9"/>
-        <v>6</v>
+        <f t="shared" si="13"/>
+        <v>5</v>
       </c>
       <c r="I47">
-        <f t="shared" si="10"/>
-        <v>2.375</v>
+        <f t="shared" si="14"/>
+        <v>2.3125</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" t="str">
-        <f t="shared" si="4"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84</v>
+        <f t="shared" si="8"/>
+        <v>0.00, 0.39, 0.77, 1.16, 1.54, 1.93, 2.31, 2.70</v>
       </c>
       <c r="B48" s="12">
-        <f t="shared" si="5"/>
-        <v>2.8365150964252184</v>
+        <f t="shared" si="9"/>
+        <v>2.7007966707589404</v>
       </c>
       <c r="C48" s="12">
-        <f t="shared" si="6"/>
-        <v>2.1913469568461488</v>
+        <f t="shared" si="10"/>
+        <v>2.1818200555934966</v>
       </c>
       <c r="D48" s="12">
-        <f t="shared" si="7"/>
-        <v>1.6129203489476731</v>
+        <f t="shared" si="11"/>
+        <v>1.7581656758666036</v>
       </c>
       <c r="F48" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>2</v>
       </c>
       <c r="G48">
-        <f t="shared" si="9"/>
-        <v>13</v>
+        <f t="shared" si="13"/>
+        <v>11</v>
       </c>
       <c r="I48">
-        <f t="shared" si="10"/>
-        <v>2.8125</v>
+        <f t="shared" si="14"/>
+        <v>2.6875</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" t="str">
-        <f t="shared" si="4"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24</v>
+        <f t="shared" si="8"/>
+        <v>0.00, 0.39, 0.77, 1.16, 1.54, 1.93, 2.31, 2.70, 3.09</v>
       </c>
       <c r="B49" s="12">
-        <f t="shared" si="5"/>
-        <v>3.2417315387716781</v>
+        <f t="shared" si="9"/>
+        <v>3.0866247665816462</v>
       </c>
       <c r="C49" s="12">
-        <f t="shared" si="6"/>
-        <v>2.5043965221098845</v>
+        <f t="shared" si="10"/>
+        <v>2.4935086349639959</v>
       </c>
       <c r="D49" s="12">
-        <f t="shared" si="7"/>
-        <v>1.8433375416544835</v>
+        <f t="shared" si="11"/>
+        <v>2.009332200990404</v>
       </c>
       <c r="F49" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="G49">
-        <f t="shared" si="9"/>
-        <v>3</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="I49">
-        <f t="shared" si="10"/>
-        <v>3.1875</v>
+        <f t="shared" si="14"/>
+        <v>3.0625</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" t="str">
-        <f t="shared" si="4"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24, 3.65</v>
+        <f t="shared" si="8"/>
+        <v>0.00, 0.39, 0.77, 1.16, 1.54, 1.93, 2.31, 2.70, 3.09, 3.47</v>
       </c>
       <c r="B50" s="12">
-        <f t="shared" si="5"/>
-        <v>3.6469479811181378</v>
+        <f t="shared" si="9"/>
+        <v>3.472452862404352</v>
       </c>
       <c r="C50" s="12">
-        <f t="shared" si="6"/>
-        <v>2.8174460873736202</v>
+        <f t="shared" si="10"/>
+        <v>2.8051972143344952</v>
       </c>
       <c r="D50" s="12">
-        <f t="shared" si="7"/>
-        <v>2.0737547343612941</v>
+        <f t="shared" si="11"/>
+        <v>2.2604987261142044</v>
       </c>
       <c r="F50" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="G50">
-        <f t="shared" si="9"/>
-        <v>10</v>
+        <f t="shared" si="13"/>
+        <v>7</v>
       </c>
       <c r="I50">
-        <f t="shared" si="10"/>
-        <v>3.625</v>
+        <f t="shared" si="14"/>
+        <v>3.4375</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" t="str">
-        <f t="shared" si="4"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24, 3.65, 4.05</v>
+        <f t="shared" si="8"/>
+        <v>0.00, 0.39, 0.77, 1.16, 1.54, 1.93, 2.31, 2.70, 3.09, 3.47, 3.86</v>
       </c>
       <c r="B51" s="12">
-        <f t="shared" si="5"/>
-        <v>4.0521644234645979</v>
+        <f t="shared" si="9"/>
+        <v>3.8582809582270579</v>
       </c>
       <c r="C51" s="12">
-        <f t="shared" si="6"/>
-        <v>3.130495652637356</v>
+        <f t="shared" si="10"/>
+        <v>3.1168857937049945</v>
       </c>
       <c r="D51" s="12">
-        <f t="shared" si="7"/>
-        <v>2.3041719270681047</v>
+        <f t="shared" si="11"/>
+        <v>2.5116652512380049</v>
       </c>
       <c r="F51" s="13">
-        <f t="shared" si="8"/>
-        <v>4</v>
+        <f t="shared" si="12"/>
+        <v>3</v>
       </c>
       <c r="G51">
-        <f t="shared" si="9"/>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>13</v>
       </c>
       <c r="I51">
-        <f t="shared" si="10"/>
-        <v>4</v>
+        <f t="shared" si="14"/>
+        <v>3.8125</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" t="str">
-        <f t="shared" si="4"/>
-        <v>0.00, 0.41, 0.81, 1.22, 1.62, 2.03, 2.43, 2.84, 3.24, 3.65, 4.05, 4.46</v>
+        <f t="shared" si="8"/>
+        <v>0.00, 0.39, 0.77, 1.16, 1.54, 1.93, 2.31, 2.70, 3.09, 3.47, 3.86, 4.24</v>
       </c>
       <c r="B52" s="12">
-        <f t="shared" si="5"/>
-        <v>4.4573808658110581</v>
+        <f t="shared" si="9"/>
+        <v>4.2441090540497637</v>
       </c>
       <c r="C52" s="12">
-        <f t="shared" si="6"/>
-        <v>3.4435452179010917</v>
+        <f t="shared" si="10"/>
+        <v>3.4285743730754938</v>
       </c>
       <c r="D52" s="12">
-        <f t="shared" si="7"/>
-        <v>2.5345891197749153</v>
+        <f t="shared" si="11"/>
+        <v>2.7628317763618053</v>
       </c>
       <c r="F52" s="13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="G52">
-        <f t="shared" si="9"/>
-        <v>7</v>
+        <f t="shared" si="13"/>
+        <v>3</v>
       </c>
       <c r="I52">
-        <f t="shared" si="10"/>
-        <v>4.4375</v>
+        <f t="shared" si="14"/>
+        <v>4.1875</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B53" s="12">
-        <f t="shared" si="5"/>
-        <v>4.8625973081575182</v>
+        <f t="shared" si="9"/>
+        <v>4.6299371498724691</v>
       </c>
       <c r="C53" s="12">
-        <f t="shared" si="6"/>
-        <v>3.7565947831648274</v>
+        <f t="shared" si="10"/>
+        <v>3.7402629524459932</v>
       </c>
       <c r="D53" s="12">
-        <f t="shared" si="7"/>
-        <v>2.7650063124817259</v>
+        <f t="shared" si="11"/>
+        <v>3.0139983014856058</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B54" s="12">
-        <f t="shared" si="5"/>
-        <v>5.2678137505039784</v>
+        <f t="shared" si="9"/>
+        <v>5.0157652456951745</v>
       </c>
       <c r="C54" s="12">
-        <f t="shared" si="6"/>
-        <v>4.0696443484285627</v>
+        <f t="shared" si="10"/>
+        <v>4.0519515318164929</v>
       </c>
       <c r="D54" s="12">
-        <f t="shared" si="7"/>
-        <v>2.9954235051885365</v>
+        <f t="shared" si="11"/>
+        <v>3.2651648266094062</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B55" s="12">
-        <f t="shared" si="5"/>
-        <v>5.6730301928504385</v>
+        <f t="shared" si="9"/>
+        <v>5.4015933415178798</v>
       </c>
       <c r="C55" s="12">
-        <f t="shared" si="6"/>
-        <v>4.3826939136922984</v>
+        <f t="shared" si="10"/>
+        <v>4.3636401111869922</v>
       </c>
       <c r="D55" s="12">
-        <f t="shared" si="7"/>
-        <v>3.2258406978953471</v>
+        <f t="shared" si="11"/>
+        <v>3.5163313517332067</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B56" s="12">
-        <f t="shared" si="5"/>
-        <v>6.0782466351968987</v>
+        <f t="shared" si="9"/>
+        <v>5.7874214373405852</v>
       </c>
       <c r="C56" s="12">
-        <f t="shared" si="6"/>
-        <v>4.6957434789560342</v>
+        <f t="shared" si="10"/>
+        <v>4.6753286905574916</v>
       </c>
       <c r="D56" s="12">
-        <f t="shared" si="7"/>
-        <v>3.4562578906021577</v>
+        <f t="shared" si="11"/>
+        <v>3.7674978768570071</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B57" s="12">
-        <f t="shared" si="5"/>
-        <v>6.4834630775433588</v>
+        <f t="shared" si="9"/>
+        <v>6.1732495331632906</v>
       </c>
       <c r="C57" s="12">
-        <f t="shared" si="6"/>
-        <v>5.0087930442197699</v>
+        <f t="shared" si="10"/>
+        <v>4.9870172699279909</v>
       </c>
       <c r="D57" s="12">
-        <f t="shared" si="7"/>
-        <v>3.6866750833089683</v>
+        <f t="shared" si="11"/>
+        <v>4.018664401980808</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B58" s="12">
-        <f t="shared" si="5"/>
-        <v>6.888679519889819</v>
+        <f t="shared" si="9"/>
+        <v>6.559077628985996</v>
       </c>
       <c r="C58" s="12">
-        <f t="shared" si="6"/>
-        <v>5.3218426094835056</v>
+        <f t="shared" si="10"/>
+        <v>5.2987058492984902</v>
       </c>
       <c r="D58" s="12">
-        <f t="shared" si="7"/>
-        <v>3.9170922760157789</v>
+        <f t="shared" si="11"/>
+        <v>4.2698309271046089</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B59" s="12">
-        <f t="shared" si="5"/>
-        <v>7.2938959622362791</v>
+        <f t="shared" si="9"/>
+        <v>6.9449057248087014</v>
       </c>
       <c r="C59" s="12">
-        <f t="shared" si="6"/>
-        <v>5.6348921747472414</v>
+        <f t="shared" si="10"/>
+        <v>5.6103944286689895</v>
       </c>
       <c r="D59" s="12">
-        <f t="shared" si="7"/>
-        <v>4.1475094687225891</v>
+        <f t="shared" si="11"/>
+        <v>4.5209974522284098</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B60" s="12">
-        <f t="shared" si="5"/>
-        <v>7.6991124045827393</v>
+        <f t="shared" si="9"/>
+        <v>7.3307338206314068</v>
       </c>
       <c r="C60" s="12">
-        <f t="shared" si="6"/>
-        <v>5.9479417400109771</v>
+        <f t="shared" si="10"/>
+        <v>5.9220830080394888</v>
       </c>
       <c r="D60" s="12">
-        <f t="shared" si="7"/>
-        <v>4.3779266614293997</v>
+        <f t="shared" si="11"/>
+        <v>4.7721639773522107</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="B61" s="12">
-        <f t="shared" ref="B61" si="11">B60+$D$36</f>
-        <v>8.1043288469291994</v>
+        <f t="shared" ref="B61" si="15">B60+$D$36</f>
+        <v>7.7165619164541122</v>
       </c>
       <c r="C61" s="12">
-        <f t="shared" ref="C61" si="12">C60+$D$37</f>
-        <v>6.2609913052747128</v>
+        <f t="shared" ref="C61" si="16">C60+$D$37</f>
+        <v>6.2337715874099882</v>
       </c>
       <c r="D61" s="12">
-        <f t="shared" ref="D61" si="13">D60+$D$38</f>
-        <v>4.6083438541362103</v>
+        <f t="shared" ref="D61" si="17">D60+$D$38</f>
+        <v>5.0233305024760115</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.45">
@@ -3750,44 +3893,50 @@
         <v>15.967105496833609</v>
       </c>
       <c r="F64" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>0</v>
       </c>
       <c r="B65" s="13">
-        <f>B66/$B$64</f>
-        <v>1.0002021665610414</v>
+        <v>1</v>
       </c>
       <c r="C65" t="str">
         <f>"0x"&amp;DEC2HEX(B65,2)</f>
         <v>0x01</v>
       </c>
+      <c r="D65" s="16">
+        <f>B65/$B$67</f>
+        <v>3.9215686274509803E-3</v>
+      </c>
       <c r="F65" s="4" t="str">
         <f>"    "&amp;C65&amp;",    // .display_intensity = "&amp;TEXT(A65,"0")</f>
         <v xml:space="preserve">    0x01,    // .display_intensity = 0</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>1</v>
       </c>
       <c r="B66" s="13">
-        <f>B67/$B$64</f>
-        <v>15.970333511641689</v>
+        <v>16</v>
       </c>
       <c r="C66" t="str">
-        <f t="shared" ref="C66:C67" si="14">"0x"&amp;DEC2HEX(B66,2)</f>
-        <v>0x0F</v>
+        <f t="shared" ref="C66:C67" si="18">"0x"&amp;DEC2HEX(B66,2)</f>
+        <v>0x10</v>
+      </c>
+      <c r="D66" s="16">
+        <f>B66/$B$67</f>
+        <v>6.2745098039215685E-2</v>
       </c>
       <c r="F66" s="4" t="str">
-        <f t="shared" ref="F66:F67" si="15">"    "&amp;C66&amp;",    // .display_intensity = "&amp;TEXT(A66,"0")</f>
-        <v xml:space="preserve">    0x0F,    // .display_intensity = 1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+        <f t="shared" ref="F66:F67" si="19">"    "&amp;C66&amp;",    // .display_intensity = "&amp;TEXT(A66,"0")</f>
+        <v xml:space="preserve">    0x10,    // .display_intensity = 1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>2</v>
       </c>
@@ -3795,20 +3944,57 @@
         <v>255</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>0xFF</v>
       </c>
+      <c r="D67" s="16">
+        <f>B67/$B$67</f>
+        <v>1</v>
+      </c>
       <c r="F67" s="4" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v xml:space="preserve">    0xFF,    // .display_intensity = 2</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="F68" s="4" t="s">
         <v>121</v>
       </c>
     </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F70" t="str">
+        <f>TEXT(D65,"0.0%")</f>
+        <v>0.4%</v>
+      </c>
+      <c r="G70" t="str">
+        <f>F70</f>
+        <v>0.4%</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F71" t="str">
+        <f>TEXT(D66,"0.0%")</f>
+        <v>6.3%</v>
+      </c>
+      <c r="G71" t="str">
+        <f>G70&amp;", "&amp;F71</f>
+        <v>0.4%, 6.3%</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="F72" t="str">
+        <f>TEXT(D67,"0.0%")</f>
+        <v>100.0%</v>
+      </c>
+      <c r="G72" t="str">
+        <f>G71&amp;", "&amp;F72</f>
+        <v>0.4%, 6.3%, 100.0%</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L14:R20">
+    <sortCondition ref="L14:L20"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
@@ -4181,7 +4367,7 @@
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.45">
       <c r="D2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.45">
@@ -4251,7 +4437,7 @@
     </row>
     <row r="4" spans="2:19" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>

</xml_diff>